<commit_message>
updating my spelling errors
</commit_message>
<xml_diff>
--- a/cv/cv_pubs.xlsx
+++ b/cv/cv_pubs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Harrisburg University/Websites/cv markdown/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Harrisburg University/Websites/github web/content/cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2134" documentId="10_ncr:8100000_{6AA46C81-726B-5D40-B419-5CCBBC6537F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{5A964149-6082-9F41-B86F-C1C5468B5A75}"/>
+  <xr:revisionPtr revIDLastSave="2135" documentId="10_ncr:8100000_{6AA46C81-726B-5D40-B419-5CCBBC6537F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{61EFCB59-772A-3D42-A57E-81D5AAFAABD9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1323,9 +1323,6 @@
     <t>Invited talk for Central High School Psychology Club  Springfield, MO</t>
   </si>
   <si>
-    <t>nvited talk for the KME Math Honor’s Society at Missouri State University: Springfield, MO</t>
-  </si>
-  <si>
     <t>Spoken presentation at the annual meeting of the Psychonomic Society Seattle, WA</t>
   </si>
   <si>
@@ -2645,6 +2642,9 @@
   </si>
   <si>
     <t>Data Analytics Summit V, Harrisburg, PA</t>
+  </si>
+  <si>
+    <t>Invited talk for the KME Math Honor’s Society at Missouri State University: Springfield, MO</t>
   </si>
 </sst>
 </file>
@@ -3553,9 +3553,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C173" sqref="C173"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="44.1640625" defaultRowHeight="16"/>
@@ -3643,13 +3643,13 @@
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="J2" s="1">
         <v>2018</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="L2" s="1">
         <v>46227693</v>
@@ -3667,7 +3667,7 @@
         <v>189</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="34">
@@ -3675,13 +3675,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>211</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>182</v>
@@ -3711,7 +3711,7 @@
         <v>189</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="34">
@@ -3719,13 +3719,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="J4" s="1">
         <v>2017</v>
@@ -3763,7 +3763,7 @@
         <v>80</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>261</v>
@@ -3813,13 +3813,13 @@
         <v>64</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="J6" s="1">
         <v>2018</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="L6" s="1">
         <v>46227698</v>
@@ -3837,7 +3837,7 @@
         <v>199</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="51">
@@ -3845,13 +3845,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="J7" s="1">
         <v>2017</v>
@@ -3875,7 +3875,7 @@
         <v>189</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="34">
@@ -3883,19 +3883,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>96</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="J8" s="1">
         <v>2018</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="L8" s="1">
         <v>46227701</v>
@@ -3913,7 +3913,7 @@
         <v>189</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="51">
@@ -3921,19 +3921,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="J9" s="1">
         <v>2017</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="L9" s="1">
         <v>46227688</v>
@@ -3951,7 +3951,7 @@
         <v>189</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="34">
@@ -3959,13 +3959,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>146</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="J10" s="1">
         <v>2019</v>
@@ -3986,7 +3986,7 @@
         <v>189</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="34">
@@ -4000,7 +4000,7 @@
         <v>132</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="J11" s="1">
         <v>2017</v>
@@ -4024,7 +4024,7 @@
         <v>189</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="34">
@@ -4032,19 +4032,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>83</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="J12" s="1">
         <v>2018</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="L12" s="1">
         <v>46227700</v>
@@ -4062,7 +4062,7 @@
         <v>189</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="34">
@@ -4070,13 +4070,13 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D13" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
@@ -4085,7 +4085,7 @@
         <v>2019</v>
       </c>
       <c r="K13" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L13">
         <v>52212308</v>
@@ -4103,7 +4103,7 @@
         <v>199</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="51">
@@ -4111,13 +4111,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="J14" s="1">
         <v>2018</v>
@@ -4141,7 +4141,7 @@
         <v>189</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="34">
@@ -4149,13 +4149,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J15" s="1">
         <v>2017</v>
@@ -4179,7 +4179,7 @@
         <v>199</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="34">
@@ -4193,7 +4193,7 @@
         <v>136</v>
       </c>
       <c r="E16" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="J16" s="1">
         <v>2018</v>
@@ -4214,7 +4214,7 @@
         <v>199</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="34">
@@ -4222,19 +4222,19 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="J17" s="1">
         <v>2018</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="L17" s="1">
         <v>46227699</v>
@@ -4252,7 +4252,7 @@
         <v>189</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="34">
@@ -4272,7 +4272,7 @@
         <v>2018</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="L18" s="1">
         <v>46227697</v>
@@ -4304,13 +4304,13 @@
         <v>121</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="J19" s="1">
         <v>2018</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="L19" s="1">
         <v>46227703</v>
@@ -4336,13 +4336,13 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D20" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -4352,7 +4352,7 @@
         <v>2019</v>
       </c>
       <c r="K20" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="L20">
         <v>53070092</v>
@@ -4370,7 +4370,7 @@
         <v>189</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="34">
@@ -4431,7 +4431,7 @@
         <v>97</v>
       </c>
       <c r="E22" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>98</v>
@@ -4443,7 +4443,7 @@
         <v>4</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J22" s="1">
         <v>2011</v>
@@ -4467,7 +4467,7 @@
         <v>199</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="51">
@@ -4531,7 +4531,7 @@
         <v>119</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>89</v>
@@ -4552,7 +4552,7 @@
         <v>120</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>183</v>
@@ -4578,10 +4578,10 @@
         <v>172</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>67</v>
@@ -4593,7 +4593,7 @@
         <v>4</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="J25" s="1">
         <v>2012</v>
@@ -4617,7 +4617,7 @@
         <v>199</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="34">
@@ -4631,7 +4631,7 @@
         <v>252</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>74</v>
@@ -4681,7 +4681,7 @@
         <v>196</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>10</v>
@@ -4728,7 +4728,7 @@
         <v>222</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>21</v>
@@ -4778,7 +4778,7 @@
         <v>32</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>33</v>
@@ -4790,7 +4790,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J29" s="1">
         <v>2013</v>
@@ -4814,7 +4814,7 @@
         <v>199</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="51">
@@ -4828,7 +4828,7 @@
         <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>39</v>
@@ -4840,7 +4840,7 @@
         <v>4</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J30" s="1">
         <v>2013</v>
@@ -4864,7 +4864,7 @@
         <v>199</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="34">
@@ -4878,7 +4878,7 @@
         <v>51</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>123</v>
@@ -4899,7 +4899,7 @@
         <v>52</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>183</v>
@@ -4928,7 +4928,7 @@
         <v>70</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>71</v>
@@ -4978,7 +4978,7 @@
         <v>122</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>123</v>
@@ -4999,7 +4999,7 @@
         <v>124</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>183</v>
@@ -5028,7 +5028,7 @@
         <v>25</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>26</v>
@@ -5078,7 +5078,7 @@
         <v>56</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>57</v>
@@ -5096,10 +5096,10 @@
         <v>2014</v>
       </c>
       <c r="K35" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>661</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>183</v>
@@ -5114,7 +5114,7 @@
         <v>199</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="51">
@@ -5128,10 +5128,10 @@
         <v>61</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G36" s="1">
         <v>118</v>
@@ -5140,7 +5140,7 @@
         <v>2</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="J36" s="1">
         <v>2014</v>
@@ -5164,7 +5164,7 @@
         <v>199</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="51">
@@ -5178,7 +5178,7 @@
         <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>89</v>
@@ -5190,7 +5190,7 @@
         <v>3</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="J37" s="1">
         <v>2014</v>
@@ -5214,7 +5214,7 @@
         <v>199</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="34">
@@ -5225,7 +5225,7 @@
         <v>113</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>242</v>
@@ -5272,13 +5272,13 @@
         <v>145</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G39" s="1">
         <v>44</v>
@@ -5287,7 +5287,7 @@
         <v>2</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J39" s="1">
         <v>2015</v>
@@ -5319,10 +5319,10 @@
         <v>171</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E40" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>86</v>
@@ -5334,7 +5334,7 @@
         <v>3</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J40" s="1">
         <v>2015</v>
@@ -5358,7 +5358,7 @@
         <v>199</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="68">
@@ -5372,7 +5372,7 @@
         <v>226</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>227</v>
@@ -5422,7 +5422,7 @@
         <v>84</v>
       </c>
       <c r="E42" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>116</v>
@@ -5434,7 +5434,7 @@
         <v>12</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J42" s="1">
         <v>2016</v>
@@ -5458,7 +5458,7 @@
         <v>199</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="43" spans="1:17" ht="51">
@@ -5472,7 +5472,7 @@
         <v>106</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>283</v>
@@ -5493,7 +5493,7 @@
         <v>107</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="M43" s="1" t="s">
         <v>183</v>
@@ -5519,7 +5519,7 @@
         <v>112</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>21</v>
@@ -5537,7 +5537,7 @@
         <v>2016</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="L44" s="1">
         <v>30745623</v>
@@ -5569,7 +5569,7 @@
         <v>128</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>33</v>
@@ -5619,10 +5619,10 @@
         <v>54</v>
       </c>
       <c r="E46" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G46" s="1">
         <v>22</v>
@@ -5631,7 +5631,7 @@
         <v>182</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="J46" s="1">
         <v>2016</v>
@@ -5655,7 +5655,7 @@
         <v>199</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="51">
@@ -5666,10 +5666,10 @@
         <v>44</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E47" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>116</v>
@@ -5681,7 +5681,7 @@
         <v>7</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="J47" s="1">
         <v>2017</v>
@@ -5705,7 +5705,7 @@
         <v>199</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="34">
@@ -5716,10 +5716,10 @@
         <v>103</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>86</v>
@@ -5731,7 +5731,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J48" s="1">
         <v>2017</v>
@@ -5755,7 +5755,7 @@
         <v>199</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="17">
@@ -5772,7 +5772,7 @@
         <v>9</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>26</v>
@@ -5825,7 +5825,7 @@
         <v>159</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>261</v>
@@ -5875,7 +5875,7 @@
         <v>31</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>186</v>
@@ -5887,13 +5887,13 @@
         <v>182</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="J51" s="1">
         <v>2018</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="L51" s="1">
         <v>46227685</v>
@@ -5922,16 +5922,16 @@
         <v>36</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="G52" s="11" t="s">
         <v>493</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>494</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>182</v>
@@ -5978,7 +5978,7 @@
         <v>148</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>46</v>
@@ -5990,7 +5990,7 @@
         <v>2</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="J53" s="1">
         <v>2018</v>
@@ -6022,13 +6022,13 @@
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>21</v>
@@ -6040,7 +6040,7 @@
         <v>182</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="J54" s="1">
         <v>2018</v>
@@ -6064,7 +6064,7 @@
         <v>189</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="55" spans="1:17" ht="17">
@@ -6072,19 +6072,19 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C55" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D55" t="s">
+        <v>668</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="F55" t="s">
         <v>669</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="F55" t="s">
-        <v>670</v>
       </c>
       <c r="G55">
         <v>10</v>
@@ -6093,13 +6093,13 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="J55">
         <v>2018</v>
       </c>
       <c r="K55" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L55">
         <v>46975449</v>
@@ -6117,7 +6117,7 @@
         <v>189</v>
       </c>
       <c r="Q55" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="34">
@@ -6125,16 +6125,16 @@
         <v>1</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>77</v>
@@ -6146,13 +6146,13 @@
         <v>3</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="J56" s="1">
         <v>2018</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>7</v>
@@ -6170,7 +6170,7 @@
         <v>199</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="34">
@@ -6187,7 +6187,7 @@
         <v>140</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>123</v>
@@ -6199,7 +6199,7 @@
         <v>6</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J57" s="1">
         <v>2018</v>
@@ -6208,7 +6208,7 @@
         <v>92</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="M57" s="1" t="s">
         <v>183</v>
@@ -6223,7 +6223,7 @@
         <v>199</v>
       </c>
       <c r="Q57" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="51">
@@ -6237,7 +6237,7 @@
         <v>133</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>104</v>
@@ -6249,7 +6249,7 @@
         <v>182</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J58" s="1">
         <v>2018</v>
@@ -6273,7 +6273,7 @@
         <v>199</v>
       </c>
       <c r="Q58" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="34">
@@ -6290,7 +6290,7 @@
         <v>282</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>110</v>
@@ -6302,13 +6302,13 @@
         <v>2</v>
       </c>
       <c r="I59" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="J59" s="1">
         <v>2019</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="L59" s="1">
         <v>44621959</v>
@@ -6340,7 +6340,7 @@
         <v>127</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>126</v>
@@ -6384,7 +6384,7 @@
         <v>1</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>236</v>
@@ -6393,7 +6393,7 @@
         <v>24</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>46</v>
@@ -6405,13 +6405,13 @@
         <v>182</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="J61" s="1">
         <v>2019</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="L61" s="1">
         <v>46227680</v>
@@ -6446,13 +6446,13 @@
         <v>12</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>288</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>182</v>
@@ -6464,7 +6464,7 @@
         <v>2019</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="L62" s="1">
         <v>46227691</v>
@@ -6493,10 +6493,10 @@
         <v>209</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>711</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>712</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>210</v>
@@ -6537,16 +6537,16 @@
         <v>1</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>50</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>123</v>
@@ -6567,7 +6567,7 @@
         <v>49</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="M64" s="1" t="s">
         <v>183</v>
@@ -6582,7 +6582,7 @@
         <v>189</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="65" spans="1:17" ht="34">
@@ -6591,14 +6591,14 @@
       </c>
       <c r="B65"/>
       <c r="C65" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D65"/>
       <c r="E65" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="F65" s="6" t="s">
         <v>841</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>842</v>
       </c>
       <c r="G65"/>
       <c r="H65"/>
@@ -6609,7 +6609,7 @@
       <c r="K65"/>
       <c r="L65"/>
       <c r="M65" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="N65" s="1" t="s">
         <v>203</v>
@@ -6621,7 +6621,7 @@
         <v>199</v>
       </c>
       <c r="Q65" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="66" spans="1:17" ht="34">
@@ -6630,14 +6630,14 @@
       </c>
       <c r="B66"/>
       <c r="C66" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D66"/>
       <c r="E66" s="1" t="s">
         <v>211</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G66"/>
       <c r="H66"/>
@@ -6648,7 +6648,7 @@
       <c r="K66"/>
       <c r="L66"/>
       <c r="M66" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="N66" s="1" t="s">
         <v>203</v>
@@ -6660,7 +6660,7 @@
         <v>199</v>
       </c>
       <c r="Q66" s="12" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="51">
@@ -6671,10 +6671,10 @@
         <v>180</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J67" s="7" t="s">
         <v>338</v>
@@ -6692,7 +6692,7 @@
         <v>189</v>
       </c>
       <c r="Q67" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="51">
@@ -6700,10 +6700,10 @@
         <v>1</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>397</v>
@@ -6724,7 +6724,7 @@
         <v>199</v>
       </c>
       <c r="Q68" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="69" spans="1:17" ht="51">
@@ -6735,7 +6735,7 @@
         <v>352</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>395</v>
@@ -6756,7 +6756,7 @@
         <v>199</v>
       </c>
       <c r="Q69" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="34">
@@ -6767,10 +6767,10 @@
         <v>371</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J70" s="7" t="s">
         <v>316</v>
@@ -6788,7 +6788,7 @@
         <v>189</v>
       </c>
       <c r="Q70" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="71" spans="1:17" ht="51">
@@ -6796,10 +6796,10 @@
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>384</v>
@@ -6820,7 +6820,7 @@
         <v>199</v>
       </c>
       <c r="Q71" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="51">
@@ -6828,10 +6828,10 @@
         <v>1</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>385</v>
@@ -6860,7 +6860,7 @@
         <v>344</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>373</v>
@@ -6881,7 +6881,7 @@
         <v>199</v>
       </c>
       <c r="Q73" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="51">
@@ -6892,7 +6892,7 @@
         <v>344</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>374</v>
@@ -6913,7 +6913,7 @@
         <v>199</v>
       </c>
       <c r="Q74" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="51">
@@ -6921,10 +6921,10 @@
         <v>1</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>382</v>
@@ -6945,7 +6945,7 @@
         <v>199</v>
       </c>
       <c r="Q75" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="34">
@@ -6997,7 +6997,7 @@
         <v>155</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>230</v>
@@ -7032,10 +7032,10 @@
         <v>157</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>233</v>
@@ -7067,7 +7067,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E79" s="7" t="s">
         <v>290</v>
@@ -7096,7 +7096,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E80" s="7" t="s">
         <v>290</v>
@@ -7120,7 +7120,7 @@
         <v>189</v>
       </c>
       <c r="Q80" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="34">
@@ -7128,7 +7128,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>290</v>
@@ -7152,7 +7152,7 @@
         <v>189</v>
       </c>
       <c r="Q81" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="34">
@@ -7160,7 +7160,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>290</v>
@@ -7184,7 +7184,7 @@
         <v>189</v>
       </c>
       <c r="Q82" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="34">
@@ -7192,7 +7192,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E83" s="7" t="s">
         <v>290</v>
@@ -7221,7 +7221,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E84" s="7" t="s">
         <v>290</v>
@@ -7245,7 +7245,7 @@
         <v>189</v>
       </c>
       <c r="Q84" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="51">
@@ -7253,7 +7253,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E85" s="7" t="s">
         <v>290</v>
@@ -7282,13 +7282,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E86" s="7" t="s">
         <v>295</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J86" s="7" t="s">
         <v>343</v>
@@ -7306,7 +7306,7 @@
         <v>199</v>
       </c>
       <c r="Q86" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="34">
@@ -7317,13 +7317,13 @@
         <v>152</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J87" s="7" t="s">
         <v>306</v>
@@ -7349,10 +7349,10 @@
         <v>1</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>391</v>
@@ -7381,7 +7381,7 @@
         <v>356</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>406</v>
@@ -7402,7 +7402,7 @@
         <v>199</v>
       </c>
       <c r="Q89" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="90" spans="1:17" ht="51">
@@ -7413,7 +7413,7 @@
         <v>349</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>388</v>
@@ -7434,7 +7434,7 @@
         <v>199</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="91" spans="1:17" ht="34">
@@ -7442,13 +7442,13 @@
         <v>1</v>
       </c>
       <c r="C91" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>505</v>
-      </c>
       <c r="E91" s="7" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>379</v>
@@ -7469,7 +7469,7 @@
         <v>199</v>
       </c>
       <c r="Q91" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="92" spans="1:17" ht="51">
@@ -7480,7 +7480,7 @@
         <v>348</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>387</v>
@@ -7506,13 +7506,13 @@
         <v>1</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J93" s="7" t="s">
         <v>310</v>
@@ -7530,7 +7530,7 @@
         <v>189</v>
       </c>
       <c r="Q93" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="94" spans="1:17" ht="34">
@@ -7541,10 +7541,10 @@
         <v>173</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>380</v>
@@ -7568,7 +7568,7 @@
         <v>199</v>
       </c>
       <c r="Q94" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="51">
@@ -7576,13 +7576,13 @@
         <v>1</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J95" s="7" t="s">
         <v>298</v>
@@ -7600,7 +7600,7 @@
         <v>199</v>
       </c>
       <c r="Q95" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="96" spans="1:17" ht="34">
@@ -7632,7 +7632,7 @@
         <v>199</v>
       </c>
       <c r="Q96" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="97" spans="1:17" ht="34">
@@ -7664,7 +7664,7 @@
         <v>199</v>
       </c>
       <c r="Q97" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="98" spans="1:17" ht="51">
@@ -7672,10 +7672,10 @@
         <v>1</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>403</v>
@@ -7696,7 +7696,7 @@
         <v>199</v>
       </c>
       <c r="Q98" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="99" spans="1:17" ht="51">
@@ -7707,7 +7707,7 @@
         <v>355</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>404</v>
@@ -7728,7 +7728,7 @@
         <v>199</v>
       </c>
       <c r="Q99" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="100" spans="1:17">
@@ -7736,17 +7736,17 @@
         <v>1</v>
       </c>
       <c r="B100" t="s">
+        <v>665</v>
+      </c>
+      <c r="C100" t="s">
         <v>666</v>
-      </c>
-      <c r="C100" t="s">
-        <v>667</v>
       </c>
       <c r="D100"/>
       <c r="E100" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F100" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="G100" s="14" t="s">
         <v>182</v>
@@ -7755,13 +7755,13 @@
         <v>182</v>
       </c>
       <c r="I100" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="J100">
         <v>2019</v>
       </c>
       <c r="K100" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="L100">
         <v>52942378</v>
@@ -7785,13 +7785,13 @@
         <v>1</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J101" s="7" t="s">
         <v>297</v>
@@ -7809,7 +7809,7 @@
         <v>189</v>
       </c>
       <c r="Q101" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="102" spans="1:17" ht="34">
@@ -7817,7 +7817,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>294</v>
@@ -7846,13 +7846,13 @@
         <v>1</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>290</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J103" s="7" t="s">
         <v>337</v>
@@ -7870,7 +7870,7 @@
         <v>189</v>
       </c>
       <c r="Q103" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="104" spans="1:17" ht="34">
@@ -7878,7 +7878,7 @@
         <v>1</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>290</v>
@@ -7910,7 +7910,7 @@
         <v>149</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E105" s="7" t="s">
         <v>290</v>
@@ -7937,7 +7937,7 @@
         <v>189</v>
       </c>
       <c r="Q105" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="106" spans="1:17" ht="34">
@@ -7945,7 +7945,7 @@
         <v>1</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E106" s="7" t="s">
         <v>290</v>
@@ -7969,7 +7969,7 @@
         <v>189</v>
       </c>
       <c r="Q106" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="107" spans="1:17" ht="34">
@@ -7977,7 +7977,7 @@
         <v>1</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>290</v>
@@ -8001,7 +8001,7 @@
         <v>189</v>
       </c>
       <c r="Q107" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="108" spans="1:17" ht="34">
@@ -8012,7 +8012,7 @@
         <v>163</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E108" s="7" t="s">
         <v>290</v>
@@ -8039,7 +8039,7 @@
         <v>189</v>
       </c>
       <c r="Q108" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="109" spans="1:17" ht="51">
@@ -8050,7 +8050,7 @@
         <v>360</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F109" s="6" t="s">
         <v>410</v>
@@ -8071,7 +8071,7 @@
         <v>199</v>
       </c>
       <c r="Q109" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="110" spans="1:17" ht="51">
@@ -8082,10 +8082,10 @@
         <v>372</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J110" s="7" t="s">
         <v>298</v>
@@ -8103,7 +8103,7 @@
         <v>189</v>
       </c>
       <c r="Q110" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="111" spans="1:17" ht="34">
@@ -8114,7 +8114,7 @@
         <v>354</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F111" s="6" t="s">
         <v>401</v>
@@ -8135,7 +8135,7 @@
         <v>199</v>
       </c>
       <c r="Q111" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="112" spans="1:17" ht="34">
@@ -8146,7 +8146,7 @@
         <v>354</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F112" s="6" t="s">
         <v>402</v>
@@ -8167,7 +8167,7 @@
         <v>199</v>
       </c>
       <c r="Q112" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="113" spans="1:17" ht="34">
@@ -8178,13 +8178,13 @@
         <v>165</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J113" s="7" t="s">
         <v>306</v>
@@ -8205,7 +8205,7 @@
         <v>189</v>
       </c>
       <c r="Q113" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="114" spans="1:17" ht="34">
@@ -8219,10 +8219,10 @@
         <v>367</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J114" s="7" t="s">
         <v>300</v>
@@ -8243,7 +8243,7 @@
         <v>189</v>
       </c>
       <c r="Q114" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="115" spans="1:17" ht="34">
@@ -8251,22 +8251,22 @@
         <v>1</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D115" t="s">
         <v>146</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J115" s="7" t="s">
         <v>308</v>
       </c>
       <c r="K115" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="L115">
         <v>46227690</v>
@@ -8284,7 +8284,7 @@
         <v>189</v>
       </c>
       <c r="Q115" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="116" spans="1:17" ht="51">
@@ -8295,10 +8295,10 @@
         <v>368</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J116" s="7" t="s">
         <v>318</v>
@@ -8316,7 +8316,7 @@
         <v>189</v>
       </c>
       <c r="Q116" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="117" spans="1:17" ht="51">
@@ -8324,10 +8324,10 @@
         <v>1</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F117" s="6" t="s">
         <v>390</v>
@@ -8348,7 +8348,7 @@
         <v>189</v>
       </c>
       <c r="Q117" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="118" spans="1:17" ht="34">
@@ -8356,13 +8356,13 @@
         <v>1</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J118" s="7" t="s">
         <v>340</v>
@@ -8380,7 +8380,7 @@
         <v>189</v>
       </c>
       <c r="Q118" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="119" spans="1:17" ht="34">
@@ -8420,10 +8420,10 @@
         <v>370</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J120" s="7" t="s">
         <v>316</v>
@@ -8441,7 +8441,7 @@
         <v>189</v>
       </c>
       <c r="Q120" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="121" spans="1:17" ht="34">
@@ -8449,13 +8449,13 @@
         <v>1</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J121" s="7" t="s">
         <v>338</v>
@@ -8473,7 +8473,7 @@
         <v>189</v>
       </c>
       <c r="Q121" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="122" spans="1:17" ht="51">
@@ -8484,7 +8484,7 @@
         <v>358</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F122" s="6" t="s">
         <v>408</v>
@@ -8505,7 +8505,7 @@
         <v>199</v>
       </c>
       <c r="Q122" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="123" spans="1:17" ht="51">
@@ -8516,7 +8516,7 @@
         <v>359</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F123" s="6" t="s">
         <v>409</v>
@@ -8537,7 +8537,7 @@
         <v>199</v>
       </c>
       <c r="Q123" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="124" spans="1:17" ht="34">
@@ -8548,7 +8548,7 @@
         <v>345</v>
       </c>
       <c r="E124" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F124" s="6" t="s">
         <v>378</v>
@@ -8569,7 +8569,7 @@
         <v>199</v>
       </c>
       <c r="Q124" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="125" spans="1:17" ht="34">
@@ -8586,7 +8586,7 @@
         <v>115</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>123</v>
@@ -8604,7 +8604,7 @@
         <v>2019</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="L125" s="1">
         <v>46227696</v>
@@ -8630,7 +8630,7 @@
         <v>1</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E126" s="7" t="s">
         <v>290</v>
@@ -8662,10 +8662,10 @@
         <v>366</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F127" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J127" s="7" t="s">
         <v>316</v>
@@ -8683,7 +8683,7 @@
         <v>189</v>
       </c>
       <c r="Q127" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="128" spans="1:17" ht="34">
@@ -8697,7 +8697,7 @@
         <v>290</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J128" s="7" t="s">
         <v>334</v>
@@ -8720,7 +8720,7 @@
         <v>1</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E129" s="7" t="s">
         <v>291</v>
@@ -8752,7 +8752,7 @@
         <v>346</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F130" s="6" t="s">
         <v>381</v>
@@ -8773,7 +8773,7 @@
         <v>199</v>
       </c>
       <c r="Q130" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="131" spans="1:17" ht="34">
@@ -8781,13 +8781,13 @@
         <v>1</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J131" s="7" t="s">
         <v>338</v>
@@ -8805,7 +8805,7 @@
         <v>189</v>
       </c>
       <c r="Q131" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="132" spans="1:17" ht="34">
@@ -8813,13 +8813,13 @@
         <v>1</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J132" s="7" t="s">
         <v>297</v>
@@ -8837,7 +8837,7 @@
         <v>189</v>
       </c>
       <c r="Q132" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="133" spans="1:17" ht="34">
@@ -8845,13 +8845,13 @@
         <v>1</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J133" s="7" t="s">
         <v>338</v>
@@ -8869,7 +8869,7 @@
         <v>189</v>
       </c>
       <c r="Q133" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="134" spans="1:17" ht="34">
@@ -8883,10 +8883,10 @@
         <v>369</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J134" s="7" t="s">
         <v>339</v>
@@ -8907,7 +8907,7 @@
         <v>189</v>
       </c>
       <c r="Q134" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="135" spans="1:17" ht="51">
@@ -8918,7 +8918,7 @@
         <v>353</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="F135" s="6" t="s">
         <v>396</v>
@@ -8944,7 +8944,7 @@
         <v>1</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E136" s="7" t="s">
         <v>290</v>
@@ -8968,7 +8968,7 @@
         <v>189</v>
       </c>
       <c r="Q136" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="137" spans="1:17" ht="34">
@@ -8979,10 +8979,10 @@
         <v>161</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="F137" s="6" t="s">
         <v>398</v>
@@ -9014,10 +9014,10 @@
         <v>162</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E138" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F138" s="6" t="s">
         <v>399</v>
@@ -9041,7 +9041,7 @@
         <v>199</v>
       </c>
       <c r="Q138" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="139" spans="1:17" ht="34">
@@ -9052,13 +9052,13 @@
         <v>170</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E139" s="7" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F139" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J139" s="7" t="s">
         <v>309</v>
@@ -9079,7 +9079,7 @@
         <v>189</v>
       </c>
       <c r="Q139" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="140" spans="1:17" ht="34">
@@ -9087,10 +9087,10 @@
         <v>1</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E140" s="7" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F140" s="6" t="s">
         <v>411</v>
@@ -9116,10 +9116,10 @@
         <v>1</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E141" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F141" s="6" t="s">
         <v>405</v>
@@ -9140,7 +9140,7 @@
         <v>199</v>
       </c>
       <c r="Q141" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="142" spans="1:17" ht="102">
@@ -9154,7 +9154,7 @@
         <v>350</v>
       </c>
       <c r="E142" s="7" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F142" s="6" t="s">
         <v>389</v>
@@ -9183,10 +9183,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E143" s="7" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F143" s="6" t="s">
         <v>407</v>
@@ -9207,7 +9207,7 @@
         <v>199</v>
       </c>
       <c r="Q143" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="144" spans="1:17" ht="34">
@@ -9215,7 +9215,7 @@
         <v>1</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E144" s="7" t="s">
         <v>290</v>
@@ -9239,7 +9239,7 @@
         <v>199</v>
       </c>
       <c r="Q144" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="145" spans="1:17" ht="34">
@@ -9247,10 +9247,10 @@
         <v>1</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E145" s="7" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F145" s="6" t="s">
         <v>378</v>
@@ -9271,7 +9271,7 @@
         <v>189</v>
       </c>
       <c r="Q145" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="146" spans="1:17" ht="51">
@@ -9279,10 +9279,10 @@
         <v>1</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E146" s="7" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F146" s="6" t="s">
         <v>400</v>
@@ -9303,7 +9303,7 @@
         <v>199</v>
       </c>
       <c r="Q146" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="147" spans="1:17" ht="34">
@@ -9311,10 +9311,10 @@
         <v>1</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E147" s="7" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F147" s="6" t="s">
         <v>386</v>
@@ -9335,7 +9335,7 @@
         <v>199</v>
       </c>
       <c r="Q147" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="148" spans="1:17" ht="51">
@@ -9343,13 +9343,13 @@
         <v>1</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E148" s="7" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F148" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J148" s="7" t="s">
         <v>341</v>
@@ -9372,13 +9372,13 @@
         <v>1</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E149" s="7" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F149" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J149" s="7" t="s">
         <v>302</v>
@@ -9396,7 +9396,7 @@
         <v>189</v>
       </c>
       <c r="Q149" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="150" spans="1:17" ht="34">
@@ -9410,7 +9410,7 @@
         <v>347</v>
       </c>
       <c r="E150" s="7" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F150" s="6" t="s">
         <v>383</v>
@@ -9442,7 +9442,7 @@
         <v>357</v>
       </c>
       <c r="E151" s="7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F151" s="6" t="s">
         <v>406</v>
@@ -9463,7 +9463,7 @@
         <v>199</v>
       </c>
       <c r="Q151" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="152" spans="1:17" ht="34">
@@ -9477,7 +9477,7 @@
         <v>290</v>
       </c>
       <c r="F152" s="6" t="s">
-        <v>430</v>
+        <v>870</v>
       </c>
       <c r="J152" s="7" t="s">
         <v>336</v>
@@ -9495,7 +9495,7 @@
         <v>199</v>
       </c>
       <c r="Q152" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="153" spans="1:17" ht="34">
@@ -9506,13 +9506,13 @@
         <v>167</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E153" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F153" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="J153" s="7" t="s">
         <v>296</v>
@@ -9533,7 +9533,7 @@
         <v>199</v>
       </c>
       <c r="Q153" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="154" spans="1:17" customFormat="1" ht="34">
@@ -9542,14 +9542,14 @@
       </c>
       <c r="B154" s="1"/>
       <c r="C154" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D154" s="1"/>
       <c r="E154" s="7" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F154" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
@@ -9572,7 +9572,7 @@
         <v>189</v>
       </c>
       <c r="Q154" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="155" spans="1:17" customFormat="1" ht="34">
@@ -9581,10 +9581,10 @@
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="D155" t="s">
         <v>577</v>
-      </c>
-      <c r="D155" t="s">
-        <v>578</v>
       </c>
       <c r="E155" s="7" t="s">
         <v>290</v>
@@ -9613,7 +9613,7 @@
         <v>199</v>
       </c>
       <c r="Q155" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="156" spans="1:17" customFormat="1" ht="51">
@@ -9622,14 +9622,14 @@
       </c>
       <c r="B156" s="1"/>
       <c r="C156" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D156" s="1"/>
       <c r="E156" s="7" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F156" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
@@ -9652,7 +9652,7 @@
         <v>189</v>
       </c>
       <c r="Q156" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="157" spans="1:17" customFormat="1" ht="34">
@@ -9661,7 +9661,7 @@
       </c>
       <c r="B157" s="1"/>
       <c r="C157" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D157" s="1"/>
       <c r="E157" s="7" t="s">
@@ -9691,7 +9691,7 @@
         <v>189</v>
       </c>
       <c r="Q157" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="158" spans="1:17" customFormat="1" ht="34">
@@ -9703,7 +9703,7 @@
         <v>361</v>
       </c>
       <c r="D158" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E158" s="7" t="s">
         <v>293</v>
@@ -9732,7 +9732,7 @@
         <v>189</v>
       </c>
       <c r="Q158" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="159" spans="1:17" customFormat="1" ht="34">
@@ -9741,7 +9741,7 @@
       </c>
       <c r="B159" s="1"/>
       <c r="C159" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D159" s="1"/>
       <c r="E159" s="7" t="s">
@@ -9819,10 +9819,10 @@
       </c>
       <c r="D161" s="1"/>
       <c r="E161" s="7" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F161" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
@@ -9845,7 +9845,7 @@
         <v>199</v>
       </c>
       <c r="Q161" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="162" spans="1:17" customFormat="1" ht="34">
@@ -9854,7 +9854,7 @@
       </c>
       <c r="B162" s="1"/>
       <c r="C162" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D162" s="1"/>
       <c r="E162" s="7" t="s">
@@ -9884,7 +9884,7 @@
         <v>189</v>
       </c>
       <c r="Q162" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="163" spans="1:17" customFormat="1" ht="51">
@@ -9892,16 +9892,16 @@
         <v>1</v>
       </c>
       <c r="C163" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="E163" s="7" t="s">
         <v>810</v>
       </c>
-      <c r="E163" s="7" t="s">
+      <c r="F163" s="6" t="s">
         <v>811</v>
       </c>
-      <c r="F163" s="6" t="s">
+      <c r="J163" s="7" t="s">
         <v>812</v>
-      </c>
-      <c r="J163" s="7" t="s">
-        <v>813</v>
       </c>
       <c r="M163" s="1" t="s">
         <v>219</v>
@@ -9916,7 +9916,7 @@
         <v>189</v>
       </c>
       <c r="Q163" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="164" spans="1:17" customFormat="1" ht="85">
@@ -9924,16 +9924,16 @@
         <v>1</v>
       </c>
       <c r="C164" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="F164" s="6" t="s">
         <v>816</v>
       </c>
-      <c r="E164" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="F164" s="6" t="s">
+      <c r="J164" s="7" t="s">
         <v>817</v>
-      </c>
-      <c r="J164" s="7" t="s">
-        <v>818</v>
       </c>
       <c r="M164" s="1" t="s">
         <v>219</v>
@@ -9953,17 +9953,17 @@
         <v>1</v>
       </c>
       <c r="C165" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E165" s="7" t="s">
         <v>819</v>
-      </c>
-      <c r="E165" s="7" t="s">
-        <v>820</v>
       </c>
       <c r="F165" s="6" t="s">
         <v>378</v>
       </c>
       <c r="G165" s="14"/>
       <c r="J165" s="7" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="M165" s="1" t="s">
         <v>219</v>
@@ -9978,7 +9978,7 @@
         <v>199</v>
       </c>
       <c r="Q165" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="166" spans="1:17" customFormat="1" ht="34">
@@ -9986,16 +9986,16 @@
         <v>1</v>
       </c>
       <c r="C166" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="E166" s="1" t="s">
         <v>821</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>822</v>
       </c>
       <c r="F166" s="6" t="s">
         <v>378</v>
       </c>
       <c r="J166" s="7" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="M166" s="1" t="s">
         <v>219</v>
@@ -10010,7 +10010,7 @@
         <v>189</v>
       </c>
       <c r="Q166" s="2" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="167" spans="1:17" customFormat="1" ht="51">
@@ -10018,16 +10018,16 @@
         <v>1</v>
       </c>
       <c r="C167" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="F167" s="6" t="s">
         <v>824</v>
       </c>
-      <c r="E167" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="F167" s="6" t="s">
+      <c r="J167" s="7" t="s">
         <v>825</v>
-      </c>
-      <c r="J167" s="7" t="s">
-        <v>826</v>
       </c>
       <c r="M167" s="1" t="s">
         <v>219</v>
@@ -10042,7 +10042,7 @@
         <v>199</v>
       </c>
       <c r="Q167" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="168" spans="1:17" customFormat="1" ht="34">
@@ -10050,16 +10050,16 @@
         <v>1</v>
       </c>
       <c r="C168" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E168" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="E168" s="1" t="s">
+      <c r="F168" s="6" t="s">
         <v>829</v>
       </c>
-      <c r="F168" s="6" t="s">
+      <c r="J168" s="7" t="s">
         <v>830</v>
-      </c>
-      <c r="J168" s="7" t="s">
-        <v>831</v>
       </c>
       <c r="M168" s="1" t="s">
         <v>219</v>
@@ -10079,16 +10079,16 @@
         <v>1</v>
       </c>
       <c r="C169" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="E169" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="E169" s="1" t="s">
+      <c r="F169" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="F169" s="6" t="s">
+      <c r="J169" s="7" t="s">
         <v>834</v>
-      </c>
-      <c r="J169" s="7" t="s">
-        <v>835</v>
       </c>
       <c r="M169" s="1" t="s">
         <v>219</v>
@@ -10103,7 +10103,7 @@
         <v>199</v>
       </c>
       <c r="Q169" s="2" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="170" spans="1:17" customFormat="1" ht="51">
@@ -10111,16 +10111,16 @@
         <v>1</v>
       </c>
       <c r="C170" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="E170" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="E170" s="1" t="s">
+      <c r="F170" s="6" t="s">
         <v>838</v>
       </c>
-      <c r="F170" s="6" t="s">
-        <v>839</v>
-      </c>
       <c r="J170" s="7" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="M170" s="1" t="s">
         <v>219</v>
@@ -10140,16 +10140,16 @@
         <v>1</v>
       </c>
       <c r="B171" t="s">
+        <v>854</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="F171" s="6" t="s">
         <v>855</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>853</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>854</v>
-      </c>
-      <c r="F171" s="6" t="s">
-        <v>856</v>
       </c>
       <c r="G171" t="s">
         <v>182</v>
@@ -10176,7 +10176,7 @@
         <v>189</v>
       </c>
       <c r="Q171" s="12" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="172" spans="1:17" customFormat="1" ht="51">
@@ -10184,16 +10184,16 @@
         <v>1</v>
       </c>
       <c r="B172" t="s">
+        <v>860</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="E172" s="1" t="s">
         <v>861</v>
       </c>
-      <c r="C172" s="1" t="s">
-        <v>865</v>
-      </c>
-      <c r="E172" s="1" t="s">
+      <c r="F172" s="6" t="s">
         <v>862</v>
-      </c>
-      <c r="F172" s="6" t="s">
-        <v>863</v>
       </c>
       <c r="G172" t="s">
         <v>182</v>
@@ -10225,16 +10225,16 @@
         <v>1</v>
       </c>
       <c r="B173" s="6" t="s">
+        <v>866</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="E173" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="C173" s="1" t="s">
-        <v>866</v>
-      </c>
-      <c r="E173" s="1" t="s">
+      <c r="F173" s="6" t="s">
         <v>868</v>
-      </c>
-      <c r="F173" s="6" t="s">
-        <v>869</v>
       </c>
       <c r="G173" t="s">
         <v>182</v>
@@ -10266,16 +10266,16 @@
         <v>1</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>211</v>
       </c>
       <c r="F174" s="6" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="J174" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="M174" s="1" t="s">
         <v>219</v>

</xml_diff>

<commit_message>
updated cv and website
</commit_message>
<xml_diff>
--- a/cv/cv_pubs.xlsx
+++ b/cv/cv_pubs.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/GitHub/Websites/cv markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D72BF12-84C8-2245-A01E-601C774E3D32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B30644F-8D9E-D745-A69C-D6A7DEDB59C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cv_pubs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cv_pubs!$A$1:$Q$192</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cv_pubs!$A$1:$Q$206</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="1043">
   <si>
     <t>title</t>
   </si>
@@ -2067,9 +2067,6 @@
     <t>https://osf.io/5qy7v</t>
   </si>
   <si>
-    <t>7Frjd3zlGBUC, 3_LpOwP6eMYC</t>
-  </si>
-  <si>
     <t>How metacognitive awareness relates to overconfidence in interval judgments</t>
   </si>
   <si>
@@ -2505,9 +2502,6 @@
     <t>Poster presentation for the Annual Meeting of the Association for Psychological Science, Washington, D.C.</t>
   </si>
   <si>
-    <t>MOTE: Measure of the Effect}: Package to assist in effect size calculations and their confidence intervals</t>
-  </si>
-  <si>
     <t>Buchanan, E.M., Gillenwaters, A., Scofield, J.E., \&amp; Valentine, K.D.</t>
   </si>
   <si>
@@ -2556,9 +2550,6 @@
     <t xml:space="preserve">SAGE Research Methods Datasets Part 2 </t>
   </si>
   <si>
-    <t>xm0LlTxljI0C; wyM6WWKXmoIC</t>
-  </si>
-  <si>
     <t>46227694, 56962138</t>
   </si>
   <si>
@@ -2637,9 +2628,6 @@
     <t>natZJ_-F0IUC</t>
   </si>
   <si>
-    <t>PsyArXiv</t>
-  </si>
-  <si>
     <t>VRfTbSk87rEC</t>
   </si>
   <si>
@@ -2709,9 +2697,6 @@
     <t>22716735, 57294613</t>
   </si>
   <si>
-    <t>RMgMIBzvq-4C, WWeOtg8bX_EC</t>
-  </si>
-  <si>
     <t>12273821, 57294601</t>
   </si>
   <si>
@@ -2874,9 +2859,6 @@
     <t>59816012, 65055132</t>
   </si>
   <si>
-    <t>9shLKfS_uJEC, eH23hyXCXa4C</t>
-  </si>
-  <si>
     <t>hNSvKAmkeYkC, I8rxH6phXEkC, g8uWPOAv7ggC</t>
   </si>
   <si>
@@ -2983,6 +2965,201 @@
   </si>
   <si>
     <t>https://osf.io/86vms</t>
+  </si>
+  <si>
+    <t>Advances in Methods and Practices in Psychological Science</t>
+  </si>
+  <si>
+    <t>Applied Neuropsychology: Adult</t>
+  </si>
+  <si>
+    <t>193--206</t>
+  </si>
+  <si>
+    <t>623--633</t>
+  </si>
+  <si>
+    <t>41--53</t>
+  </si>
+  <si>
+    <t>1--27</t>
+  </si>
+  <si>
+    <t>ofz524</t>
+  </si>
+  <si>
+    <t>10.1093/ofid/ofz524</t>
+  </si>
+  <si>
+    <t>registered</t>
+  </si>
+  <si>
+    <t>10.1080/23279095.2020.1735388</t>
+  </si>
+  <si>
+    <t>Meaning, social support, and resilience as predictors of posttraumatic growth: A study of the Louisiana flooding of August 2016</t>
+  </si>
+  <si>
+    <t>Examining daily-level associations between nightly alcohol use and next-day valued behavior in college students</t>
+  </si>
+  <si>
+    <t>Pavlacic, J. M., Weber, M. C., Torres, V. A., Schulenberg, S. E., \&amp; Buchanan, E. M.</t>
+  </si>
+  <si>
+    <t>Trajectories of psychological functioning and pandemic preparedness for students quarantined during the COVID-19 pandemic</t>
+  </si>
+  <si>
+    <t>Grant presentation accepted at the 45th Annual Natural Hazards workshop and Research Meeting of the Natural Hazards Center, Boulder, Colorado.</t>
+  </si>
+  <si>
+    <t>2020, July</t>
+  </si>
+  <si>
+    <t>Pavlacic, J. M., Schulenberg, S. E., \&amp; Buchanan, E. M.</t>
+  </si>
+  <si>
+    <t>Meaning, purpose, and experiential avoidance as predictors of valued behavior: A daily diary study</t>
+  </si>
+  <si>
+    <t>In S. C. Hayes, Discussant, New Research Directions at the Interface of Values and Psychological Flexibility. Symposium accepted to the 54th Annual Convention of the Association for Behavioral and Cognitive Therapies, Philadelphia, Pennsylvania</t>
+  </si>
+  <si>
+    <t>2020, November</t>
+  </si>
+  <si>
+    <t>Pavlacic, J. M., Buchanan, E. M., McCaslin, S. E., \&amp; Schulenberg, S. E.</t>
+  </si>
+  <si>
+    <t>A systematic review of posttraumatic stress and resilience trajectories and covariates in veterans and service members</t>
+  </si>
+  <si>
+    <t>Poster accepted to the 54th Annual Convention of the Association for Behavioral and Cognitive Therapies, Philadelphia, Pennsylvania</t>
+  </si>
+  <si>
+    <t>Unconference: Here’s the PSA!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buchanan, E.M., Wagge, J., Miller, J., Primbs, M., \&amp; Steltenpohl, C. </t>
+  </si>
+  <si>
+    <t>Hackathon: Contribute, Curate, or Code the Open Scholarship Knowledge Base</t>
+  </si>
+  <si>
+    <t>Buchanan, E.M., Henninger, F., \&amp; Clyburne-Sherin, A.</t>
+  </si>
+  <si>
+    <t>Unconference: Towards a Community-Built Open Scholarship Knowledge Base</t>
+  </si>
+  <si>
+    <t>Clyburne-Sherin, A., Buchanan, E.M., \&amp; Henninger, F.</t>
+  </si>
+  <si>
+    <t>Hackathon: Collaborative Open Science Research with Undergraduates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Levitan, C., Wagge, J., Buchanan, E.M., \&amp; Benjamin, J. </t>
+  </si>
+  <si>
+    <t>2020, June</t>
+  </si>
+  <si>
+    <t>https://osf.io/b3hp8/</t>
+  </si>
+  <si>
+    <t>https://osf.io/576pd/</t>
+  </si>
+  <si>
+    <t>https://osf.io/tem7k/</t>
+  </si>
+  <si>
+    <t>https://osf.io/d4q95/</t>
+  </si>
+  <si>
+    <t>10.1080/07448481.2020.1785473</t>
+  </si>
+  <si>
+    <t>Pavlacic, J. M., Dixon, L. J., Schulenberg, S. E., \&amp; Buchanan, E. M.</t>
+  </si>
+  <si>
+    <t>Journal of American College Health</t>
+  </si>
+  <si>
+    <t>10.1037/ort0000464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boullion, G. Q., Pavlacic, J. M., Schulenberg, S. E., Buchanan, E. M., \&amp; Steger, M. F. </t>
+  </si>
+  <si>
+    <t>American Journal of Orthopsychiatry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power simulations for linguistic norm data collection </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buchanan, E. M., Valentine, K. D., Maxwell, N. P., Taylor, J. E., \&amp; Montefinese, M. </t>
+  </si>
+  <si>
+    <t>Spoken presentation for the Annual Meeting of the Psychonomic Society, Austin, TX</t>
+  </si>
+  <si>
+    <t>Unconference presentation for the Annual Meeting of the Society for the Improvement of Psychological Science, Victoria, Canada</t>
+  </si>
+  <si>
+    <t>Hackathon presentation for the Annual Meeting of the Society for the Improvement of Psychological Science, Victoria, Canada</t>
+  </si>
+  <si>
+    <t>Testing the assumption of model similarity across languages</t>
+  </si>
+  <si>
+    <t>Grim II, P. A. \&amp; Buchanan, E.M.</t>
+  </si>
+  <si>
+    <t>Spoken presentation for the Annual Meeting of the Society for Computation in Psychology, Austin TX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buchanan, E.M. \&amp; Korn, J. </t>
+  </si>
+  <si>
+    <t>300-310</t>
+  </si>
+  <si>
+    <t>QaSi33NTfwYC</t>
+  </si>
+  <si>
+    <t>Vno172sVVMwC</t>
+  </si>
+  <si>
+    <t>Ej9njvOgR2oC</t>
+  </si>
+  <si>
+    <t>9shLKfS_uJEC, eH23hyXCXa4C, xyvS_IvSCKsC</t>
+  </si>
+  <si>
+    <t>7Frjd3zlGBUC, 3_LpOwP6eMYC, 3lUAU8Oskd0C</t>
+  </si>
+  <si>
+    <t>JH5k92_tO-AC</t>
+  </si>
+  <si>
+    <t>RMgMIBzvq-4C, WWeOtg8bX_EC, vVJNg6_NJEsC</t>
+  </si>
+  <si>
+    <t>xm0LlTxljI0C; wyM6WWKXmoIC, KI9T_ytC6pkC</t>
+  </si>
+  <si>
+    <t>60iIaj97TE0C</t>
+  </si>
+  <si>
+    <t>Moderators of the Relationship between Implicit and Explicit Measures of Evaluation and Identification</t>
+  </si>
+  <si>
+    <t>Schmidt, K., Buchanan, E. M., \&amp; Hall, B.</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Social Psychology</t>
+  </si>
+  <si>
+    <t>MOTE: Measure of the Effect: Package to assist in effect size calculations and their confidence intervals</t>
   </si>
 </sst>
 </file>
@@ -3926,11 +4103,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q195"/>
+  <dimension ref="A1:Q206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q197" sqref="Q197"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="44.1640625" defaultRowHeight="16"/>
@@ -4021,7 +4198,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>25</v>
@@ -4033,7 +4210,7 @@
         <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>922</v>
+        <v>917</v>
       </c>
       <c r="J2" s="1">
         <v>2019</v>
@@ -4042,7 +4219,7 @@
         <v>7</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>180</v>
@@ -4068,7 +4245,7 @@
         <v>178</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>432</v>
@@ -4103,7 +4280,7 @@
         <v>193</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -4150,7 +4327,7 @@
         <v>450</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>393</v>
@@ -4188,7 +4365,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>284</v>
@@ -4200,16 +4377,16 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="J6" s="1">
         <v>2019</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>180</v>
@@ -4235,7 +4412,7 @@
         <v>348</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>391</v>
@@ -4267,7 +4444,7 @@
         <v>367</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>445</v>
@@ -4305,7 +4482,7 @@
         <v>157</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>257</v>
@@ -4349,16 +4526,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D10" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="E10" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="F10" t="s">
-        <v>868</v>
+        <v>76</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -4367,7 +4544,7 @@
         <v>2019</v>
       </c>
       <c r="K10" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="L10">
         <v>59592572</v>
@@ -4376,7 +4553,7 @@
         <v>180</v>
       </c>
       <c r="N10" t="s">
-        <v>201</v>
+        <v>986</v>
       </c>
       <c r="O10" t="s">
         <v>184</v>
@@ -4385,7 +4562,7 @@
         <v>186</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="34">
@@ -4396,10 +4573,10 @@
         <v>206</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>698</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>207</v>
@@ -4443,10 +4620,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>380</v>
@@ -4475,19 +4652,19 @@
         <v>1.5</v>
       </c>
       <c r="B13" t="s">
-        <v>942</v>
+        <v>937</v>
       </c>
       <c r="C13" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="D13" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="F13" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="G13" t="s">
         <v>179</v>
@@ -4502,10 +4679,10 @@
         <v>2019</v>
       </c>
       <c r="K13" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="L13" t="s">
-        <v>946</v>
+        <v>941</v>
       </c>
       <c r="M13" t="s">
         <v>180</v>
@@ -4520,7 +4697,7 @@
         <v>186</v>
       </c>
       <c r="Q13" s="11" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="51">
@@ -4531,7 +4708,7 @@
         <v>455</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>381</v>
@@ -4552,7 +4729,7 @@
         <v>196</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="34">
@@ -4563,7 +4740,7 @@
         <v>340</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>369</v>
@@ -4595,7 +4772,7 @@
         <v>340</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>370</v>
@@ -4627,7 +4804,7 @@
         <v>457</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>378</v>
@@ -4635,6 +4812,9 @@
       <c r="J17" s="7" t="s">
         <v>300</v>
       </c>
+      <c r="K17" t="s">
+        <v>1030</v>
+      </c>
       <c r="M17" s="1" t="s">
         <v>216</v>
       </c>
@@ -4656,15 +4836,17 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="D18" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="E18" t="s">
-        <v>882</v>
-      </c>
-      <c r="F18"/>
+        <v>878</v>
+      </c>
+      <c r="F18" t="s">
+        <v>978</v>
+      </c>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
@@ -4672,7 +4854,7 @@
         <v>2019</v>
       </c>
       <c r="K18" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="L18">
         <v>57710195</v>
@@ -4681,7 +4863,7 @@
         <v>180</v>
       </c>
       <c r="N18" t="s">
-        <v>201</v>
+        <v>986</v>
       </c>
       <c r="O18" t="s">
         <v>184</v>
@@ -4690,7 +4872,7 @@
         <v>186</v>
       </c>
       <c r="Q18" s="11" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="34">
@@ -4783,19 +4965,19 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="J21" s="1">
         <v>2018</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="L21" s="1">
         <v>46227693</v>
@@ -4824,7 +5006,7 @@
         <v>218</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>20</v>
@@ -4874,7 +5056,7 @@
         <v>222</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>223</v>
@@ -4924,7 +5106,7 @@
         <v>153</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>226</v>
@@ -4962,7 +5144,7 @@
         <v>460</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>229</v>
@@ -5018,7 +5200,7 @@
         <v>186</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="34">
@@ -5146,7 +5328,7 @@
         <v>186</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="34">
@@ -5163,7 +5345,7 @@
         <v>23</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>45</v>
@@ -5175,13 +5357,13 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>923</v>
+        <v>918</v>
       </c>
       <c r="J31" s="1">
         <v>2019</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="L31" s="1">
         <v>46227680</v>
@@ -5213,7 +5395,7 @@
         <v>24</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>25</v>
@@ -5263,7 +5445,7 @@
         <v>29</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="J33" s="1">
         <v>2017</v>
@@ -5301,7 +5483,7 @@
         <v>30</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>183</v>
@@ -5319,7 +5501,7 @@
         <v>2018</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="L34" s="1">
         <v>46227685</v>
@@ -5401,7 +5583,7 @@
         <v>186</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="34">
@@ -5415,7 +5597,7 @@
         <v>31</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>32</v>
@@ -5497,7 +5679,7 @@
         <v>473</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>426</v>
@@ -5521,7 +5703,7 @@
         <v>186</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="51">
@@ -5532,7 +5714,7 @@
         <v>481</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>387</v>
@@ -5553,7 +5735,7 @@
         <v>196</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="85">
@@ -5562,20 +5744,20 @@
       </c>
       <c r="B41"/>
       <c r="C41" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D41"/>
       <c r="E41" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="G41"/>
       <c r="H41"/>
       <c r="I41"/>
       <c r="J41" s="7" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K41"/>
       <c r="L41"/>
@@ -5592,7 +5774,7 @@
         <v>196</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="51">
@@ -5618,7 +5800,7 @@
         <v>4</v>
       </c>
       <c r="I42" t="s">
-        <v>921</v>
+        <v>916</v>
       </c>
       <c r="J42" s="1">
         <v>2019</v>
@@ -5653,7 +5835,7 @@
         <v>352</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>402</v>
@@ -5688,7 +5870,7 @@
         <v>490</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>489</v>
@@ -5724,7 +5906,7 @@
         <v>196</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="34">
@@ -5733,11 +5915,11 @@
       </c>
       <c r="B45"/>
       <c r="C45" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D45"/>
       <c r="E45" s="7" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>374</v>
@@ -5746,7 +5928,7 @@
       <c r="H45"/>
       <c r="I45"/>
       <c r="J45" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="K45"/>
       <c r="L45"/>
@@ -5763,7 +5945,7 @@
         <v>196</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="34">
@@ -5772,22 +5954,24 @@
       </c>
       <c r="B46"/>
       <c r="C46" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D46"/>
       <c r="E46" s="1" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>975</v>
+        <v>969</v>
       </c>
       <c r="G46"/>
       <c r="H46"/>
       <c r="I46"/>
       <c r="J46" s="7" t="s">
-        <v>815</v>
-      </c>
-      <c r="K46"/>
+        <v>814</v>
+      </c>
+      <c r="K46" t="s">
+        <v>1031</v>
+      </c>
       <c r="L46"/>
       <c r="M46" s="1" t="s">
         <v>216</v>
@@ -5802,7 +5986,7 @@
         <v>196</v>
       </c>
       <c r="Q46" t="s">
-        <v>958</v>
+        <v>952</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="51">
@@ -5813,7 +5997,7 @@
         <v>345</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>384</v>
@@ -5848,7 +6032,7 @@
         <v>37</v>
       </c>
       <c r="E48" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>38</v>
@@ -5892,7 +6076,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>208</v>
@@ -5942,7 +6126,7 @@
         <v>498</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>375</v>
@@ -5974,7 +6158,7 @@
         <v>344</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>383</v>
@@ -5995,7 +6179,7 @@
         <v>196</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="51">
@@ -6056,7 +6240,7 @@
         <v>588</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>441</v>
@@ -6094,7 +6278,7 @@
         <v>146</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>45</v>
@@ -6106,7 +6290,7 @@
         <v>2</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="J54" s="1">
         <v>2018</v>
@@ -6144,7 +6328,7 @@
         <v>500</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>376</v>
@@ -6185,7 +6369,7 @@
         <v>49</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>121</v>
@@ -6197,7 +6381,7 @@
         <v>4</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
       <c r="J56" s="1">
         <v>2019</v>
@@ -6206,7 +6390,7 @@
         <v>48</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>180</v>
@@ -6232,7 +6416,7 @@
         <v>502</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>427</v>
@@ -6267,7 +6451,7 @@
         <v>50</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>121</v>
@@ -6288,7 +6472,7 @@
         <v>51</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>180</v>
@@ -6318,10 +6502,10 @@
       </c>
       <c r="D59"/>
       <c r="E59" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F59" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G59" s="23">
         <v>27</v>
@@ -6330,7 +6514,7 @@
         <v>6</v>
       </c>
       <c r="I59" t="s">
-        <v>956</v>
+        <v>950</v>
       </c>
       <c r="J59">
         <v>2019</v>
@@ -6354,7 +6538,7 @@
         <v>196</v>
       </c>
       <c r="Q59" s="2" t="s">
-        <v>899</v>
+        <v>894</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="34">
@@ -6429,7 +6613,7 @@
         <v>505</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>399</v>
@@ -6461,7 +6645,7 @@
         <v>351</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>400</v>
@@ -6496,7 +6680,7 @@
         <v>53</v>
       </c>
       <c r="E64" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>593</v>
@@ -6546,7 +6730,7 @@
         <v>55</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>56</v>
@@ -6593,7 +6777,7 @@
         <v>597</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>433</v>
@@ -6646,7 +6830,7 @@
         <v>186</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="34">
@@ -6710,7 +6894,7 @@
         <v>186</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="34">
@@ -6861,7 +7045,7 @@
         <v>356</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>406</v>
@@ -6890,37 +7074,37 @@
         <v>1.5</v>
       </c>
       <c r="B75" t="s">
-        <v>943</v>
+        <v>938</v>
       </c>
       <c r="C75" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="D75" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="E75" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>908</v>
-      </c>
-      <c r="G75" t="s">
-        <v>179</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>179</v>
+        <v>903</v>
+      </c>
+      <c r="G75">
+        <v>33</v>
+      </c>
+      <c r="H75" s="1">
+        <v>2</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>275</v>
+        <v>980</v>
       </c>
       <c r="J75">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K75" t="s">
-        <v>944</v>
+        <v>939</v>
       </c>
       <c r="L75" t="s">
-        <v>945</v>
+        <v>940</v>
       </c>
       <c r="M75" t="s">
         <v>180</v>
@@ -6935,7 +7119,7 @@
         <v>196</v>
       </c>
       <c r="Q75" s="11" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="34">
@@ -6949,7 +7133,7 @@
         <v>59</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>20</v>
@@ -6999,7 +7183,7 @@
         <v>60</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>608</v>
@@ -7044,20 +7228,20 @@
       </c>
       <c r="B78"/>
       <c r="C78" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D78"/>
       <c r="E78" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G78"/>
       <c r="H78"/>
       <c r="I78"/>
       <c r="J78" s="7" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="K78"/>
       <c r="L78"/>
@@ -7074,31 +7258,39 @@
         <v>196</v>
       </c>
       <c r="Q78" s="2" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" ht="17">
       <c r="A79" s="18">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="D79" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="E79" t="s">
-        <v>888</v>
-      </c>
-      <c r="F79"/>
-      <c r="G79"/>
-      <c r="H79"/>
-      <c r="I79"/>
+        <v>884</v>
+      </c>
+      <c r="F79" t="s">
+        <v>978</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="J79">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K79" t="s">
-        <v>947</v>
+        <v>1033</v>
       </c>
       <c r="L79">
         <v>57614693</v>
@@ -7107,7 +7299,7 @@
         <v>180</v>
       </c>
       <c r="N79" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O79" t="s">
         <v>184</v>
@@ -7116,7 +7308,7 @@
         <v>196</v>
       </c>
       <c r="Q79" s="11" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="34">
@@ -7130,13 +7322,13 @@
         <v>63</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="J80" s="1">
         <v>2018</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="L80" s="1">
         <v>46227698</v>
@@ -7162,16 +7354,16 @@
         <v>1.5</v>
       </c>
       <c r="B81" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C81" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D81" t="s">
         <v>661</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="F81" t="s">
         <v>662</v>
@@ -7183,7 +7375,7 @@
         <v>1</v>
       </c>
       <c r="I81" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="J81">
         <v>2018</v>
@@ -7207,7 +7399,7 @@
         <v>186</v>
       </c>
       <c r="Q81" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="51">
@@ -7215,7 +7407,7 @@
         <v>1.5</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>612</v>
@@ -7224,22 +7416,22 @@
         <v>65</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>179</v>
+        <v>852</v>
+      </c>
+      <c r="G82" s="1">
+        <v>49</v>
+      </c>
+      <c r="H82" s="1">
+        <v>2</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>275</v>
+        <v>981</v>
       </c>
       <c r="J82" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>64</v>
@@ -7274,7 +7466,7 @@
         <v>95</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J83" s="1">
         <v>2018</v>
@@ -7312,7 +7504,7 @@
         <v>614</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>66</v>
@@ -7333,7 +7525,7 @@
         <v>67</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="M84" s="1" t="s">
         <v>180</v>
@@ -7359,7 +7551,7 @@
         <v>368</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>448</v>
@@ -7391,7 +7583,7 @@
         <v>350</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>397</v>
@@ -7423,7 +7615,7 @@
         <v>350</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>398</v>
@@ -7452,37 +7644,37 @@
         <v>1.5</v>
       </c>
       <c r="B88" s="20" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>907</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>179</v>
+        <v>902</v>
+      </c>
+      <c r="G88" s="1">
+        <v>21</v>
+      </c>
+      <c r="H88" s="1">
+        <v>1</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>275</v>
+        <v>982</v>
       </c>
       <c r="J88" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>948</v>
+        <v>942</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>933</v>
+        <v>928</v>
       </c>
       <c r="M88" s="1" t="s">
         <v>180</v>
@@ -7511,7 +7703,7 @@
         <v>602</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>495</v>
@@ -7549,7 +7741,7 @@
         <v>69</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>70</v>
@@ -7599,7 +7791,7 @@
         <v>248</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>73</v>
@@ -7702,7 +7894,7 @@
         <v>363</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>430</v>
@@ -7743,7 +7935,7 @@
         <v>113</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>121</v>
@@ -7755,7 +7947,7 @@
         <v>4</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
       <c r="J94" s="1">
         <v>2019</v>
@@ -7793,7 +7985,7 @@
         <v>144</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>17</v>
@@ -7840,7 +8032,7 @@
         <v>144</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>437</v>
@@ -7878,7 +8070,7 @@
         <v>364</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>434</v>
@@ -7913,7 +8105,7 @@
         <v>130</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="J98" s="1">
         <v>2017</v>
@@ -7948,7 +8140,7 @@
         <v>532</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>386</v>
@@ -7983,7 +8175,7 @@
         <v>79</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>257</v>
@@ -8030,7 +8222,7 @@
         <v>628</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>440</v>
@@ -8083,7 +8275,7 @@
         <v>186</v>
       </c>
       <c r="Q102" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="103" spans="1:17" ht="34">
@@ -8094,7 +8286,7 @@
         <v>366</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>438</v>
@@ -8129,25 +8321,25 @@
         <v>82</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G104" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H104" s="1" t="s">
-        <v>179</v>
+      <c r="G104" s="1">
+        <v>25</v>
+      </c>
+      <c r="H104" s="1">
+        <v>1</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>275</v>
+        <v>983</v>
       </c>
       <c r="J104" s="1">
         <v>2019</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>678</v>
+        <v>1034</v>
       </c>
       <c r="L104" s="1">
         <v>46227700</v>
@@ -8176,7 +8368,7 @@
         <v>537</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F105" s="6" t="s">
         <v>439</v>
@@ -8211,7 +8403,7 @@
         <v>83</v>
       </c>
       <c r="E106" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>114</v>
@@ -8258,7 +8450,7 @@
         <v>354</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F107" s="6" t="s">
         <v>404</v>
@@ -8290,7 +8482,7 @@
         <v>355</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F108" s="6" t="s">
         <v>405</v>
@@ -8322,7 +8514,7 @@
         <v>341</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F109" s="6" t="s">
         <v>374</v>
@@ -8357,7 +8549,7 @@
         <v>633</v>
       </c>
       <c r="E110" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>85</v>
@@ -8378,7 +8570,7 @@
         <v>86</v>
       </c>
       <c r="L110" s="1" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="M110" s="1" t="s">
         <v>180</v>
@@ -8407,7 +8599,7 @@
         <v>87</v>
       </c>
       <c r="E111" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>88</v>
@@ -8452,14 +8644,14 @@
       </c>
       <c r="B112"/>
       <c r="C112" s="1" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D112"/>
       <c r="E112" s="1" t="s">
         <v>208</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="G112"/>
       <c r="H112"/>
@@ -8470,7 +8662,7 @@
       <c r="K112"/>
       <c r="L112"/>
       <c r="M112" s="1" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="N112" s="1" t="s">
         <v>200</v>
@@ -8482,12 +8674,15 @@
         <v>196</v>
       </c>
       <c r="Q112" s="11" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="113" spans="1:17" ht="34">
       <c r="A113" s="18">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>987</v>
       </c>
       <c r="C113" t="s">
         <v>666</v>
@@ -8496,16 +8691,25 @@
         <v>665</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>756</v>
-      </c>
-      <c r="G113"/>
-      <c r="H113"/>
-      <c r="I113"/>
+        <v>755</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="G113" t="s">
+        <v>179</v>
+      </c>
+      <c r="H113" t="s">
+        <v>179</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="J113">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K113" t="s">
-        <v>892</v>
+        <v>1036</v>
       </c>
       <c r="L113">
         <v>52212308</v>
@@ -8514,7 +8718,7 @@
         <v>180</v>
       </c>
       <c r="N113" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O113" t="s">
         <v>195</v>
@@ -8555,7 +8759,7 @@
         <v>186</v>
       </c>
       <c r="Q114" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="115" spans="1:17" ht="51">
@@ -8566,7 +8770,7 @@
         <v>362</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F115" s="6" t="s">
         <v>428</v>
@@ -8604,7 +8808,7 @@
         <v>138</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>121</v>
@@ -8672,7 +8876,7 @@
         <v>186</v>
       </c>
       <c r="Q117" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="118" spans="1:17" ht="51">
@@ -8686,7 +8890,7 @@
         <v>94</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="J118" s="1">
         <v>2018</v>
@@ -8718,17 +8922,17 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="D119"/>
       <c r="E119" s="1" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="G119" t="s">
         <v>179</v>
@@ -8736,14 +8940,14 @@
       <c r="H119" t="s">
         <v>179</v>
       </c>
-      <c r="I119" t="s">
-        <v>179</v>
+      <c r="I119" s="1" t="s">
+        <v>275</v>
       </c>
       <c r="J119">
         <v>2019</v>
       </c>
       <c r="K119" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
       <c r="L119"/>
       <c r="M119" s="1" t="s">
@@ -8759,7 +8963,7 @@
         <v>196</v>
       </c>
       <c r="Q119" s="2" t="s">
-        <v>901</v>
+        <v>896</v>
       </c>
     </row>
     <row r="120" spans="1:17" ht="34">
@@ -8768,11 +8972,11 @@
       </c>
       <c r="B120"/>
       <c r="C120" s="1" t="s">
-        <v>973</v>
+        <v>967</v>
       </c>
       <c r="D120"/>
       <c r="E120" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F120" s="6" t="s">
         <v>374</v>
@@ -8781,7 +8985,7 @@
       <c r="H120"/>
       <c r="I120"/>
       <c r="J120" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="K120"/>
       <c r="L120"/>
@@ -8798,7 +9002,7 @@
         <v>186</v>
       </c>
       <c r="Q120" s="2" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="121" spans="1:17" ht="34">
@@ -8807,14 +9011,14 @@
       </c>
       <c r="B121"/>
       <c r="C121" s="1" t="s">
-        <v>824</v>
+        <v>1042</v>
       </c>
       <c r="D121"/>
       <c r="E121" s="1" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="G121"/>
       <c r="H121"/>
@@ -8825,7 +9029,7 @@
       <c r="K121"/>
       <c r="L121"/>
       <c r="M121" s="1" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="N121" s="1" t="s">
         <v>200</v>
@@ -8837,7 +9041,7 @@
         <v>196</v>
       </c>
       <c r="Q121" s="2" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="122" spans="1:17" ht="51">
@@ -8846,20 +9050,20 @@
       </c>
       <c r="B122"/>
       <c r="C122" s="1" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D122"/>
       <c r="E122" s="7" t="s">
+        <v>796</v>
+      </c>
+      <c r="F122" s="6" t="s">
         <v>797</v>
-      </c>
-      <c r="F122" s="6" t="s">
-        <v>798</v>
       </c>
       <c r="G122"/>
       <c r="H122"/>
       <c r="I122"/>
       <c r="J122" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="K122"/>
       <c r="L122"/>
@@ -8876,7 +9080,7 @@
         <v>186</v>
       </c>
       <c r="Q122" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="123" spans="1:17" ht="51">
@@ -8890,7 +9094,7 @@
         <v>96</v>
       </c>
       <c r="E123" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>97</v>
@@ -8911,7 +9115,7 @@
         <v>98</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>893</v>
+        <v>888</v>
       </c>
       <c r="M123" s="1" t="s">
         <v>180</v>
@@ -8958,7 +9162,7 @@
         <v>196</v>
       </c>
       <c r="Q124" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="125" spans="1:17" ht="34">
@@ -8969,7 +9173,7 @@
         <v>342</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F125" s="6" t="s">
         <v>377</v>
@@ -9001,7 +9205,7 @@
         <v>539</v>
       </c>
       <c r="E126" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F126" s="6" t="s">
         <v>444</v>
@@ -9036,13 +9240,13 @@
         <v>99</v>
       </c>
       <c r="E127" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="J127" s="1">
         <v>2017</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>894</v>
+        <v>889</v>
       </c>
       <c r="L127" s="1">
         <v>46227678</v>
@@ -9074,7 +9278,7 @@
         <v>134</v>
       </c>
       <c r="E128" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="J128" s="1">
         <v>2018</v>
@@ -9106,10 +9310,10 @@
         <v>540</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>976</v>
+        <v>970</v>
       </c>
       <c r="J129" s="7" t="s">
         <v>293</v>
@@ -9138,7 +9342,7 @@
         <v>549</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F130" s="6" t="s">
         <v>431</v>
@@ -9173,7 +9377,7 @@
         <v>365</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F131" s="6" t="s">
         <v>435</v>
@@ -9208,7 +9412,7 @@
         <v>349</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F132" s="6" t="s">
         <v>392</v>
@@ -9229,7 +9433,7 @@
         <v>196</v>
       </c>
       <c r="Q132" s="2" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
     </row>
     <row r="133" spans="1:17" ht="34">
@@ -9243,7 +9447,7 @@
         <v>649</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>85</v>
@@ -9325,7 +9529,7 @@
         <v>131</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>102</v>
@@ -9375,7 +9579,7 @@
         <v>579</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F136" s="6" t="s">
         <v>394</v>
@@ -9399,7 +9603,7 @@
         <v>196</v>
       </c>
       <c r="Q136" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="137" spans="1:17" ht="34">
@@ -9413,7 +9617,7 @@
         <v>550</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F137" s="6" t="s">
         <v>395</v>
@@ -9451,7 +9655,7 @@
         <v>551</v>
       </c>
       <c r="E138" s="7" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F138" s="6" t="s">
         <v>429</v>
@@ -9490,7 +9694,7 @@
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>279</v>
@@ -9539,7 +9743,7 @@
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="7" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F140" s="6" t="s">
         <v>407</v>
@@ -9565,7 +9769,7 @@
         <v>196</v>
       </c>
       <c r="Q140" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="141" spans="1:17" customFormat="1" ht="51">
@@ -9578,7 +9782,7 @@
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="7" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F141" s="6" t="s">
         <v>401</v>
@@ -9612,16 +9816,16 @@
         <v>1</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="F142" s="6" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="G142">
         <v>81</v>
@@ -9630,13 +9834,13 @@
         <v>2</v>
       </c>
       <c r="I142" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="J142" s="7">
         <v>2019</v>
       </c>
       <c r="K142" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="L142">
         <v>57294563</v>
@@ -9654,7 +9858,7 @@
         <v>196</v>
       </c>
       <c r="Q142" s="2" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
     </row>
     <row r="143" spans="1:17" customFormat="1" ht="102">
@@ -9669,7 +9873,7 @@
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="7" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F143" s="6" t="s">
         <v>385</v>
@@ -9697,7 +9901,7 @@
         <v>196</v>
       </c>
       <c r="Q143" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="144" spans="1:17" customFormat="1" ht="51">
@@ -9710,7 +9914,7 @@
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F144" s="6" t="s">
         <v>403</v>
@@ -9788,7 +9992,7 @@
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F146" s="6" t="s">
         <v>374</v>
@@ -9831,7 +10035,7 @@
         <v>278</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>108</v>
@@ -9843,7 +10047,7 @@
         <v>2</v>
       </c>
       <c r="I147" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="J147" s="1">
         <v>2019</v>
@@ -9875,16 +10079,16 @@
         <v>1</v>
       </c>
       <c r="C148" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="E148" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="E148" s="1" t="s">
+      <c r="F148" s="6" t="s">
         <v>822</v>
       </c>
-      <c r="F148" s="6" t="s">
-        <v>823</v>
-      </c>
       <c r="J148" s="7" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="M148" s="1" t="s">
         <v>216</v>
@@ -9899,7 +10103,7 @@
         <v>196</v>
       </c>
       <c r="Q148" s="2" t="s">
-        <v>959</v>
+        <v>953</v>
       </c>
     </row>
     <row r="149" spans="1:17" customFormat="1" ht="51">
@@ -9912,7 +10116,7 @@
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F149" s="6" t="s">
         <v>396</v>
@@ -9951,7 +10155,7 @@
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="7" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F150" s="6" t="s">
         <v>382</v>
@@ -9990,7 +10194,7 @@
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="8" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>20</v>
@@ -10039,7 +10243,7 @@
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>238</v>
@@ -10088,7 +10292,7 @@
       </c>
       <c r="D153" s="1"/>
       <c r="E153" s="7" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="F153" s="6" t="s">
         <v>442</v>
@@ -10114,7 +10318,7 @@
         <v>186</v>
       </c>
       <c r="Q153" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="154" spans="1:17" customFormat="1" ht="34">
@@ -10127,7 +10331,7 @@
       </c>
       <c r="D154" s="1"/>
       <c r="E154" s="7" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="F154" s="6" t="s">
         <v>443</v>
@@ -10168,7 +10372,7 @@
         <v>57</v>
       </c>
       <c r="E155" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
@@ -10178,7 +10382,7 @@
         <v>2018</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>841</v>
+        <v>1037</v>
       </c>
       <c r="L155" s="1">
         <v>46227699</v>
@@ -10211,7 +10415,7 @@
       </c>
       <c r="D156" s="1"/>
       <c r="E156" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F156" s="6" t="s">
         <v>379</v>
@@ -10239,7 +10443,7 @@
         <v>196</v>
       </c>
       <c r="Q156" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="157" spans="1:17" ht="51">
@@ -10274,7 +10478,7 @@
         <v>115</v>
       </c>
       <c r="L157" s="1" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
       <c r="M157" s="1" t="s">
         <v>180</v>
@@ -10300,7 +10504,7 @@
         <v>353</v>
       </c>
       <c r="E158" s="7" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F158" s="6" t="s">
         <v>402</v>
@@ -10335,7 +10539,7 @@
         <v>286</v>
       </c>
       <c r="F159" s="6" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="J159" s="7" t="s">
         <v>332</v>
@@ -10373,7 +10577,7 @@
         <v>2018</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>897</v>
+        <v>892</v>
       </c>
       <c r="L160" s="1">
         <v>46227697</v>
@@ -10405,7 +10609,7 @@
         <v>526</v>
       </c>
       <c r="E161" s="7" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F161" s="6" t="s">
         <v>535</v>
@@ -10443,7 +10647,7 @@
         <v>117</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>88</v>
@@ -10493,7 +10697,7 @@
         <v>119</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J163" s="1">
         <v>2018</v>
@@ -10531,7 +10735,7 @@
         <v>120</v>
       </c>
       <c r="E164" s="8" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>121</v>
@@ -10578,7 +10782,7 @@
         <v>524</v>
       </c>
       <c r="E165" s="7" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F165" s="6" t="s">
         <v>436</v>
@@ -10643,20 +10847,20 @@
       </c>
       <c r="B167"/>
       <c r="C167" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D167"/>
       <c r="E167" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="F167" s="6" t="s">
         <v>817</v>
-      </c>
-      <c r="F167" s="6" t="s">
-        <v>818</v>
       </c>
       <c r="G167"/>
       <c r="H167"/>
       <c r="I167"/>
       <c r="J167" s="7" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="K167"/>
       <c r="L167"/>
@@ -10673,7 +10877,7 @@
         <v>196</v>
       </c>
       <c r="Q167" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="168" spans="1:17" ht="34">
@@ -10682,20 +10886,20 @@
       </c>
       <c r="B168"/>
       <c r="C168" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D168"/>
       <c r="E168" s="1" t="s">
         <v>208</v>
       </c>
       <c r="F168" s="6" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="G168"/>
       <c r="H168"/>
       <c r="I168"/>
       <c r="J168" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K168"/>
       <c r="L168"/>
@@ -10712,7 +10916,7 @@
         <v>196</v>
       </c>
       <c r="Q168" s="2" t="s">
-        <v>902</v>
+        <v>897</v>
       </c>
     </row>
     <row r="169" spans="1:17" ht="51">
@@ -10723,7 +10927,7 @@
         <v>494</v>
       </c>
       <c r="E169" s="7" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F169" s="6" t="s">
         <v>431</v>
@@ -10825,7 +11029,7 @@
         <v>125</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>124</v>
@@ -10869,17 +11073,17 @@
         <v>1</v>
       </c>
       <c r="B173" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D173"/>
       <c r="E173" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="F173" s="6" t="s">
         <v>838</v>
-      </c>
-      <c r="F173" s="6" t="s">
-        <v>840</v>
       </c>
       <c r="G173" t="s">
         <v>179</v>
@@ -10893,7 +11097,9 @@
       <c r="J173">
         <v>2019</v>
       </c>
-      <c r="K173"/>
+      <c r="K173" t="s">
+        <v>1038</v>
+      </c>
       <c r="L173"/>
       <c r="M173" s="1" t="s">
         <v>180</v>
@@ -10908,7 +11114,7 @@
         <v>186</v>
       </c>
       <c r="Q173" s="11" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="174" spans="1:17" ht="34">
@@ -10940,7 +11146,7 @@
         <v>196</v>
       </c>
       <c r="Q174" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="175" spans="1:17" ht="34">
@@ -10972,7 +11178,7 @@
         <v>186</v>
       </c>
       <c r="Q175" s="1" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="176" spans="1:17" ht="34">
@@ -10986,7 +11192,7 @@
         <v>126</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>32</v>
@@ -11033,7 +11239,7 @@
         <v>126</v>
       </c>
       <c r="E177" s="7" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F177" s="6" t="s">
         <v>446</v>
@@ -11100,7 +11306,7 @@
         <v>667</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F179"/>
       <c r="G179"/>
@@ -11142,10 +11348,10 @@
         <v>667</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F180" s="6" t="s">
-        <v>916</v>
+        <v>911</v>
       </c>
       <c r="G180"/>
       <c r="H180"/>
@@ -11176,19 +11382,19 @@
         <v>1</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
       <c r="J181" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="M181" s="1" t="s">
         <v>216</v>
@@ -11203,7 +11409,7 @@
         <v>196</v>
       </c>
       <c r="Q181" s="2" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
     </row>
     <row r="182" spans="1:17" ht="51">
@@ -11211,16 +11417,16 @@
         <v>1</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>910</v>
+        <v>905</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>911</v>
+        <v>906</v>
       </c>
       <c r="J182" s="1" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="M182" s="1" t="s">
         <v>216</v>
@@ -11235,7 +11441,7 @@
         <v>196</v>
       </c>
       <c r="Q182" s="2" t="s">
-        <v>969</v>
+        <v>963</v>
       </c>
     </row>
     <row r="183" spans="1:17" ht="51">
@@ -11243,16 +11449,16 @@
         <v>1</v>
       </c>
       <c r="C183" s="21" t="s">
-        <v>913</v>
+        <v>908</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>914</v>
+        <v>909</v>
       </c>
       <c r="F183" s="6" t="s">
-        <v>915</v>
+        <v>910</v>
       </c>
       <c r="J183" s="1" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="M183" s="1" t="s">
         <v>216</v>
@@ -11267,7 +11473,7 @@
         <v>186</v>
       </c>
       <c r="Q183" s="2" t="s">
-        <v>960</v>
+        <v>954</v>
       </c>
     </row>
     <row r="184" spans="1:17" ht="34">
@@ -11275,16 +11481,16 @@
         <v>1</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="F184" s="6" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="J184" s="1" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="M184" s="1" t="s">
         <v>216</v>
@@ -11299,7 +11505,7 @@
         <v>186</v>
       </c>
       <c r="Q184" s="2" t="s">
-        <v>961</v>
+        <v>955</v>
       </c>
     </row>
     <row r="185" spans="1:17" ht="34">
@@ -11307,16 +11513,16 @@
         <v>1</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F185" s="6" t="s">
-        <v>920</v>
+        <v>915</v>
       </c>
       <c r="J185" s="1" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="M185" s="1" t="s">
         <v>216</v>
@@ -11331,7 +11537,7 @@
         <v>196</v>
       </c>
       <c r="Q185" s="2" t="s">
-        <v>962</v>
+        <v>956</v>
       </c>
     </row>
     <row r="186" spans="1:17" ht="51">
@@ -11339,25 +11545,25 @@
         <v>1.5</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>924</v>
+        <v>919</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>925</v>
+        <v>920</v>
       </c>
       <c r="D186" t="s">
         <v>665</v>
       </c>
       <c r="E186" s="6" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>926</v>
+        <v>921</v>
       </c>
       <c r="J186" s="1" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="K186" t="s">
-        <v>927</v>
+        <v>922</v>
       </c>
       <c r="M186" s="1" t="s">
         <v>216</v>
@@ -11380,19 +11586,19 @@
         <v>1</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>928</v>
+        <v>923</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>929</v>
+        <v>924</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="J187" s="1">
         <v>2019</v>
       </c>
       <c r="K187" s="1" t="s">
-        <v>930</v>
+        <v>925</v>
       </c>
       <c r="L187">
         <v>61451311</v>
@@ -11410,7 +11616,7 @@
         <v>196</v>
       </c>
       <c r="Q187" s="2" t="s">
-        <v>931</v>
+        <v>926</v>
       </c>
     </row>
     <row r="188" spans="1:17" ht="36">
@@ -11419,13 +11625,13 @@
       </c>
       <c r="B188" s="19"/>
       <c r="C188" s="1" t="s">
-        <v>941</v>
+        <v>936</v>
       </c>
       <c r="D188" s="22" t="s">
-        <v>934</v>
+        <v>929</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
       <c r="J188" s="1">
         <v>2019</v>
@@ -11446,7 +11652,7 @@
         <v>186</v>
       </c>
       <c r="Q188" s="2" t="s">
-        <v>935</v>
+        <v>930</v>
       </c>
     </row>
     <row r="189" spans="1:17" ht="34">
@@ -11454,16 +11660,16 @@
         <v>1</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>938</v>
+        <v>933</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>937</v>
+        <v>932</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>939</v>
+        <v>934</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>940</v>
+        <v>935</v>
       </c>
       <c r="J189" s="1">
         <v>2016</v>
@@ -11492,31 +11698,31 @@
         <v>1</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>955</v>
+        <v>949</v>
       </c>
       <c r="C190" s="22" t="s">
-        <v>949</v>
+        <v>943</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>950</v>
+        <v>944</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>951</v>
-      </c>
-      <c r="G190" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H190" s="1" t="s">
-        <v>179</v>
+        <v>945</v>
+      </c>
+      <c r="G190" s="1">
+        <v>44</v>
+      </c>
+      <c r="H190" s="1">
+        <v>2</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>275</v>
+        <v>1029</v>
       </c>
       <c r="J190" s="1">
         <v>2019</v>
       </c>
       <c r="K190" t="s">
-        <v>952</v>
+        <v>946</v>
       </c>
       <c r="M190" s="1" t="s">
         <v>180</v>
@@ -11531,30 +11737,33 @@
         <v>196</v>
       </c>
       <c r="Q190" s="2" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
     </row>
     <row r="191" spans="1:17" ht="34">
       <c r="A191" s="17">
         <v>1</v>
       </c>
+      <c r="B191" s="1" t="s">
+        <v>985</v>
+      </c>
       <c r="C191" s="1" t="s">
-        <v>974</v>
+        <v>968</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>954</v>
-      </c>
-      <c r="G191" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H191" s="1" t="s">
-        <v>179</v>
+        <v>948</v>
+      </c>
+      <c r="G191" s="1">
+        <v>6</v>
+      </c>
+      <c r="H191" s="1">
+        <v>12</v>
       </c>
       <c r="I191" s="1" t="s">
-        <v>275</v>
+        <v>984</v>
       </c>
       <c r="J191" s="1">
         <v>2019</v>
@@ -11572,7 +11781,7 @@
         <v>196</v>
       </c>
       <c r="Q191" s="2" t="s">
-        <v>963</v>
+        <v>957</v>
       </c>
     </row>
     <row r="192" spans="1:17" ht="34">
@@ -11580,22 +11789,22 @@
         <v>1</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>964</v>
+        <v>958</v>
       </c>
       <c r="D192" t="s">
-        <v>965</v>
+        <v>959</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>966</v>
+        <v>960</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>967</v>
+        <v>961</v>
       </c>
       <c r="J192" s="1">
         <v>2019</v>
       </c>
       <c r="K192" t="s">
-        <v>978</v>
+        <v>972</v>
       </c>
       <c r="L192">
         <v>66133660</v>
@@ -11613,7 +11822,7 @@
         <v>196</v>
       </c>
       <c r="Q192" s="11" t="s">
-        <v>968</v>
+        <v>962</v>
       </c>
     </row>
     <row r="193" spans="1:17" ht="17">
@@ -11621,19 +11830,19 @@
         <v>1</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>980</v>
+        <v>974</v>
       </c>
       <c r="D193" s="22" t="s">
-        <v>979</v>
+        <v>973</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>981</v>
+        <v>975</v>
       </c>
       <c r="J193" s="1">
         <v>2019</v>
       </c>
       <c r="K193" t="s">
-        <v>982</v>
+        <v>976</v>
       </c>
       <c r="L193">
         <v>66565618</v>
@@ -11651,14 +11860,433 @@
         <v>196</v>
       </c>
       <c r="Q193" s="2" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="194" spans="1:17">
-      <c r="L194"/>
-    </row>
-    <row r="195" spans="1:17">
-      <c r="C195"/>
+        <v>977</v>
+      </c>
+    </row>
+    <row r="194" spans="1:17" ht="51">
+      <c r="A194" s="17">
+        <v>1</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H194" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I194" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="J194" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K194" t="s">
+        <v>1035</v>
+      </c>
+      <c r="L194">
+        <v>74750310</v>
+      </c>
+      <c r="M194" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="N194" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O194" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P194" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="195" spans="1:17" ht="51">
+      <c r="A195" s="17">
+        <v>1</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H195" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I195" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="J195" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K195" t="s">
+        <v>1032</v>
+      </c>
+      <c r="L195">
+        <v>77376584</v>
+      </c>
+      <c r="M195" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="N195" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O195" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P195" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="196" spans="1:17" ht="51">
+      <c r="A196" s="17">
+        <v>1</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="J196" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="M196" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N196" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O196" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P196" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="197" spans="1:17" ht="85">
+      <c r="A197" s="17">
+        <v>1</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="J197" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="M197" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N197" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O197" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P197" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:17" ht="51">
+      <c r="A198" s="17">
+        <v>1</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="J198" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="M198" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N198" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O198" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P198" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="199" spans="1:17" ht="51">
+      <c r="A199" s="17">
+        <v>1</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="J199" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="M199" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N199" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O199" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P199" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q199" s="1" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="200" spans="1:17" ht="51">
+      <c r="A200" s="17">
+        <v>1</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J200" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="M200" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N200" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O200" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P200" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q200" s="1" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="201" spans="1:17" ht="51">
+      <c r="A201" s="17">
+        <v>1</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="J201" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="M201" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N201" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O201" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P201" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q201" s="1" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="202" spans="1:17" ht="51">
+      <c r="A202" s="17">
+        <v>1</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J202" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="M202" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N202" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O202" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P202" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q202" s="1" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="203" spans="1:17" ht="34">
+      <c r="A203" s="17">
+        <v>1</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="J203" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="M203" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N203" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O203" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P203" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="204" spans="1:17" ht="34">
+      <c r="A204" s="17">
+        <v>1</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="J204" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="M204" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N204" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O204" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P204" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="205" spans="1:17" ht="34">
+      <c r="A205" s="17">
+        <v>1</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="J205" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="M205" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N205" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O205" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P205" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="206" spans="1:17" ht="34">
+      <c r="A206" s="17">
+        <v>1</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="J206" s="1">
+        <v>2020</v>
+      </c>
+      <c r="M206" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="N206" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="O206" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P206" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q181">

</xml_diff>

<commit_message>
updated a few small things
</commit_message>
<xml_diff>
--- a/cv/cv_pubs.xlsx
+++ b/cv/cv_pubs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/GitHub/Websites/cv markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7B8286-C845-1A45-B817-B75D4EF295BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550C8DDD-D009-564D-BD86-82527210C568}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2105" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2104" uniqueCount="1067">
   <si>
     <t>title</t>
   </si>
@@ -3226,6 +3226,12 @@
   </si>
   <si>
     <t>h168fVGZblEC</t>
+  </si>
+  <si>
+    <t>578--585</t>
+  </si>
+  <si>
+    <t>8VtEwCQfWZkC</t>
   </si>
 </sst>
 </file>
@@ -4171,9 +4177,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K123" sqref="K123"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q209" sqref="Q209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="44.1640625" defaultRowHeight="16"/>
@@ -11991,14 +11997,14 @@
       <c r="F195" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="G195" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H195" s="1" t="s">
-        <v>179</v>
+      <c r="G195" s="1">
+        <v>90</v>
+      </c>
+      <c r="H195" s="1">
+        <v>5</v>
       </c>
       <c r="I195" s="1" t="s">
-        <v>275</v>
+        <v>1065</v>
       </c>
       <c r="J195" s="1">
         <v>2020</v>
@@ -12462,6 +12468,9 @@
       </c>
       <c r="J209" s="1">
         <v>2019</v>
+      </c>
+      <c r="K209" t="s">
+        <v>1066</v>
       </c>
       <c r="M209" s="1" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
adding new pres and pubs
</commit_message>
<xml_diff>
--- a/cv/cv_pubs.xlsx
+++ b/cv/cv_pubs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/7_websites/cv_markdown_edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B67CFB-8223-CB45-BACC-861C46D5EB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6456E3B5-38C0-7944-8D96-A62B21474CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="cv_pubs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cv_pubs!$A$1:$R$245</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cv_pubs!$A$1:$R$256</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2473" uniqueCount="1266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="1313">
   <si>
     <t>title</t>
   </si>
@@ -2906,9 +2906,6 @@
     <t>Buchanan, E.M., Manley, H., Sly, J., Cady, R., Wikowsky, A., \&amp; Cunningham, A.L.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>https://osf.io/ey326</t>
   </si>
   <si>
@@ -3485,18 +3482,12 @@
     <t>https://psyarxiv.com/6s8bj</t>
   </si>
   <si>
-    <t>Discrimination, meaning, pandemic self-efficacy, and social support predict trajectories of peri-pandemic growth and resilience for marginalized university students</t>
-  </si>
-  <si>
     <t>Pavlacic, J. M., Weber, M. C., Torres, V. A., Ho, L. Y.,  Buchanan, E. M., \&amp; Schulenberg, S. E.</t>
   </si>
   <si>
     <t>https://osf.io/sevkf</t>
   </si>
   <si>
-    <t>A global test of message framing on behavioural intentions, policy support, information seeking, and experienced anxiety during the COVID-19 pandemic</t>
-  </si>
-  <si>
     <t>10.31234/osf.io/sevkf</t>
   </si>
   <si>
@@ -3818,9 +3809,6 @@
     <t>104340998, 104340998</t>
   </si>
   <si>
-    <t>8VtEwCQfWZkC, XAp-VaTZjjwC, e84hm74t-eoC, uAPFzskPt0AC, oqD4_j7ulsYC</t>
-  </si>
-  <si>
     <t>BJtnxTr0fRcC; yIeBiWEAh44C, yIeBiWEAh44C, BJtnxTr0fRcC</t>
   </si>
   <si>
@@ -3834,13 +3822,166 @@
   </si>
   <si>
     <t xml:space="preserve">xm0LlTxljI0C, wyM6WWKXmoIC, KI9T_ytC6pkC, qsWQJNntlusC </t>
+  </si>
+  <si>
+    <t>10.1007/s11136-022-03279-9</t>
+  </si>
+  <si>
+    <t>Quality of Life Research</t>
+  </si>
+  <si>
+    <t>XX-XX</t>
+  </si>
+  <si>
+    <t>Meaning, pandemic self-efficacy, social support, and discrimination predict trajectories of peri-pandemic growth and distress for international students</t>
+  </si>
+  <si>
+    <t>https://www.aggieerin.com/pubs/Pavlacic_22_PT.docx</t>
+  </si>
+  <si>
+    <t>Assessing the Effectiveness and Utility of a Mindfulness-Based Ecological Momentary Intervention</t>
+  </si>
+  <si>
+    <t>Pavlacic, J.M., Schulenberg, S.E., Witcraft, S.M., \&amp; Buchanan, E.M.</t>
+  </si>
+  <si>
+    <t>Poster presentation for the 56th annual meeting of the Association for Behavioral and Cognitive Therapies, New York, NY </t>
+  </si>
+  <si>
+    <t>2022, November</t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t>Is Priming Consistent Across Languages? Preliminary Findings from the SPAML: Semantic Priming Across Many Languages</t>
+  </si>
+  <si>
+    <t>Spoken presentation at the annual meeting of the Psychonomic Society, Boston, MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heyman, T., Buchanan, E.M., et al. </t>
+  </si>
+  <si>
+    <t>Spoken presentation for the Annual Meeting of the Society for Computation in Psychology, Boston, MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crowdsourcing Multiverse Analyses to Examine the Robustness of Research Findings </t>
+  </si>
+  <si>
+    <t>https://www.aggieerin.com/pubs/MDM_0322.pptx</t>
+  </si>
+  <si>
+    <t>Improving Patient’s Assessment of Their Migraine</t>
+  </si>
+  <si>
+    <t>2022, March</t>
+  </si>
+  <si>
+    <t>Invited spoken presentation for the Medical Decision Making Research Group at Massachusetts General Hospital</t>
+  </si>
+  <si>
+    <t>Invited spoken presentation for the University of Mississippi's clinical research students, Oxford, MS</t>
+  </si>
+  <si>
+    <t>https://www.aggieerin.com/pubs/UM_032522.pptx</t>
+  </si>
+  <si>
+    <t>A PSA on the PSA: Big Team Science with the Psychological Science Accelerator</t>
+  </si>
+  <si>
+    <t>Power to the Stimuli: Not the Effect</t>
+  </si>
+  <si>
+    <t>Invited spoken presentation for Princeton University's Statistics Research Series, Princeton, NJ</t>
+  </si>
+  <si>
+    <t>https://www.aggieerin.com/pubs/SPAML_03_29.pptx</t>
+  </si>
+  <si>
+    <t>SPAM-L: Semantic Priming Across Many Languages</t>
+  </si>
+  <si>
+    <t>Invited spoken presentation for Stanford University's brown bag series</t>
+  </si>
+  <si>
+    <t>Big Team Science Infrastructure</t>
+  </si>
+  <si>
+    <t>Invited presentation for the Big Team Science Conference 2022</t>
+  </si>
+  <si>
+    <t>2022, October</t>
+  </si>
+  <si>
+    <t>How to setup a big Team Science project within PSA</t>
+  </si>
+  <si>
+    <t>Buchanan, E. M. \&amp; Chartier, C.</t>
+  </si>
+  <si>
+    <t>Invited presentation for the Advancing Big-team Reproducible science through Increased Representation Conference 2022</t>
+  </si>
+  <si>
+    <t>2022, September</t>
+  </si>
+  <si>
+    <t>https://www.aggieerin.com/pubs/ABRIR_22.pptx</t>
+  </si>
+  <si>
+    <t>Invited presentation for the University of Utah Linguistics program</t>
+  </si>
+  <si>
+    <t>https://www.aggieerin.com/pubs/spam_open.pptx</t>
+  </si>
+  <si>
+    <t>BTS Comes for Linguistics</t>
+  </si>
+  <si>
+    <t>63--68</t>
+  </si>
+  <si>
+    <t>10.1177/1745691622110042</t>
+  </si>
+  <si>
+    <t>554–-566</t>
+  </si>
+  <si>
+    <t>101888659, 119378183</t>
+  </si>
+  <si>
+    <t>Data from an International Multi-centre Study of Statistics and Mathematics Anxieties and Related Variables in University Students (the SMARVUS Dataset)</t>
+  </si>
+  <si>
+    <t>Terry, J. et al.</t>
+  </si>
+  <si>
+    <t>l6Q3WhenKVUC</t>
+  </si>
+  <si>
+    <t>https://psyarxiv.com/au9vp/</t>
+  </si>
+  <si>
+    <t>In COVID-19 health messaging, loss framing increases anxiety with little-to-no concomitant benefits: Experimental evidence from 84 countries</t>
+  </si>
+  <si>
+    <t>1--26</t>
+  </si>
+  <si>
+    <t>u3T1itk59dMC</t>
+  </si>
+  <si>
+    <t>8VtEwCQfWZkC, XAp-VaTZjjwC, e84hm74t-eoC, uAPFzskPt0AC, oqD4_j7ulsYC, DQNrXyjhriIC</t>
+  </si>
+  <si>
+    <t>Nature Scientific Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3995,13 +4136,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="TimesNewRomanPSMT"/>
       <family val="2"/>
     </font>
     <font>
@@ -4381,7 +4515,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4429,24 +4563,33 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -4835,11 +4978,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R252"/>
+  <dimension ref="A1:R256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K87" sqref="K87"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R244" sqref="R244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="44.1640625" defaultRowHeight="16"/>
@@ -4918,7 +5061,7 @@
         <v>190</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>1197</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="34">
@@ -5777,7 +5920,7 @@
         <v>726</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>178</v>
@@ -5786,7 +5929,7 @@
         <v>178</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="J18" s="1">
         <v>2014</v>
@@ -6651,7 +6794,7 @@
         <v>15</v>
       </c>
       <c r="L35" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>179</v>
@@ -7593,7 +7736,7 @@
         <v>179</v>
       </c>
       <c r="N54" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="O54" t="s">
         <v>183</v>
@@ -7623,7 +7766,7 @@
       <c r="F55" t="s">
         <v>681</v>
       </c>
-      <c r="G55" s="22">
+      <c r="G55" s="21">
         <v>27</v>
       </c>
       <c r="H55">
@@ -7674,7 +7817,7 @@
         <v>875</v>
       </c>
       <c r="F56" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="G56"/>
       <c r="H56"/>
@@ -7692,7 +7835,7 @@
         <v>179</v>
       </c>
       <c r="N56" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="O56" t="s">
         <v>183</v>
@@ -7716,7 +7859,7 @@
         <v>832</v>
       </c>
       <c r="D57" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>833</v>
@@ -7731,13 +7874,13 @@
         <v>178</v>
       </c>
       <c r="I57" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="J57">
         <v>2019</v>
       </c>
       <c r="K57" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="L57"/>
       <c r="M57" s="1" t="s">
@@ -8005,7 +8148,7 @@
         <v>3</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="J62">
         <v>2020</v>
@@ -8039,10 +8182,10 @@
       </c>
       <c r="B63"/>
       <c r="C63" s="1" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D63" s="21" t="s">
-        <v>1052</v>
+        <v>1211</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>1051</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>803</v>
@@ -8055,7 +8198,7 @@
         <v>2019</v>
       </c>
       <c r="K63" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="L63">
         <v>78301690</v>
@@ -8073,7 +8216,7 @@
         <v>185</v>
       </c>
       <c r="Q63" s="11" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="R63" s="1"/>
     </row>
@@ -8083,13 +8226,13 @@
       </c>
       <c r="B64"/>
       <c r="C64" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D64" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="F64" s="6"/>
       <c r="G64"/>
@@ -8115,7 +8258,7 @@
         <v>185</v>
       </c>
       <c r="Q64" s="11" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="R64" s="1"/>
     </row>
@@ -8125,7 +8268,7 @@
       </c>
       <c r="B65"/>
       <c r="C65" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D65"/>
       <c r="E65" s="1" t="s">
@@ -8141,7 +8284,7 @@
         <v>2019</v>
       </c>
       <c r="K65" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="L65"/>
       <c r="M65" s="1" t="s">
@@ -8187,7 +8330,7 @@
         <v>2</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="J66" s="1">
         <v>2020</v>
@@ -8221,7 +8364,7 @@
       <c r="A67" s="16">
         <v>1.5</v>
       </c>
-      <c r="B67" s="19" t="s">
+      <c r="B67" s="18" t="s">
         <v>897</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -8243,7 +8386,7 @@
         <v>1</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="J67" s="1">
         <v>2020</v>
@@ -8299,7 +8442,7 @@
         <v>2</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="J68">
         <v>2020</v>
@@ -8411,15 +8554,15 @@
       </c>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:18" ht="36">
+    <row r="71" spans="1:18" ht="34">
       <c r="A71" s="16">
         <v>1</v>
       </c>
-      <c r="B71" s="18"/>
+      <c r="B71" s="27"/>
       <c r="C71" s="1" t="s">
         <v>931</v>
       </c>
-      <c r="D71" s="21" t="s">
+      <c r="D71" s="20" t="s">
         <v>924</v>
       </c>
       <c r="E71" s="1" t="s">
@@ -8471,13 +8614,13 @@
         <v>1</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="J72" s="1">
         <v>2019</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="L72" s="1">
         <v>46227700</v>
@@ -8527,7 +8670,7 @@
         <v>178</v>
       </c>
       <c r="I73" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="J73">
         <v>2020</v>
@@ -8557,36 +8700,42 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="34">
+    <row r="74" spans="1:18" ht="51">
       <c r="A74" s="16">
         <v>1</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>953</v>
-      </c>
-      <c r="D74" t="s">
-        <v>954</v>
+      <c r="B74" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>938</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>955</v>
+        <v>939</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>956</v>
+        <v>940</v>
+      </c>
+      <c r="G74" s="1">
+        <v>44</v>
+      </c>
+      <c r="H74" s="1">
+        <v>2</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>1021</v>
       </c>
       <c r="J74" s="1">
         <v>2019</v>
       </c>
       <c r="K74" t="s">
-        <v>967</v>
-      </c>
-      <c r="L74">
-        <v>66133660</v>
+        <v>941</v>
       </c>
       <c r="M74" s="1" t="s">
         <v>179</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O74" s="1" t="s">
         <v>194</v>
@@ -8594,42 +8743,41 @@
       <c r="P74" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q74" s="11" t="s">
-        <v>957</v>
-      </c>
-      <c r="R74" s="1"/>
-    </row>
-    <row r="75" spans="1:18" ht="51">
+      <c r="Q74" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="R74" s="8">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" ht="34">
       <c r="A75" s="16">
         <v>1</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>944</v>
-      </c>
-      <c r="C75" s="25" t="s">
-        <v>938</v>
+        <v>979</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>962</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>939</v>
+        <v>942</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>940</v>
+        <v>943</v>
       </c>
       <c r="G75" s="1">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="H75" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>1022</v>
+        <v>978</v>
       </c>
       <c r="J75" s="1">
         <v>2019</v>
       </c>
-      <c r="K75" t="s">
-        <v>941</v>
-      </c>
       <c r="M75" s="1" t="s">
         <v>179</v>
       </c>
@@ -8643,10 +8791,10 @@
         <v>195</v>
       </c>
       <c r="Q75" s="2" t="s">
-        <v>960</v>
+        <v>952</v>
       </c>
       <c r="R75" s="8">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="34">
@@ -8654,13 +8802,13 @@
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>256</v>
@@ -8672,7 +8820,7 @@
         <v>179</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="O76" s="1" t="s">
         <v>183</v>
@@ -8681,7 +8829,7 @@
         <v>185</v>
       </c>
       <c r="Q76" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R76" s="1"/>
     </row>
@@ -8689,29 +8837,32 @@
       <c r="A77" s="16">
         <v>1</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>980</v>
-      </c>
       <c r="C77" s="1" t="s">
-        <v>963</v>
+        <v>620</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>942</v>
+        <v>739</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>943</v>
-      </c>
-      <c r="G77" s="1">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>1069</v>
       </c>
       <c r="H77" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>979</v>
+        <v>1070</v>
       </c>
       <c r="J77" s="1">
-        <v>2019</v>
+        <v>2020</v>
+      </c>
+      <c r="L77" s="1">
+        <v>46227690</v>
       </c>
       <c r="M77" s="1" t="s">
         <v>179</v>
@@ -8723,101 +8874,107 @@
         <v>194</v>
       </c>
       <c r="P77" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q77" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="R77" s="8">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" ht="34">
+      <c r="A78" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="D78" t="s">
+        <v>662</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>752</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="G78">
+        <v>29</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78" t="s">
+        <v>1240</v>
+      </c>
+      <c r="J78">
+        <v>2020</v>
+      </c>
+      <c r="K78" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L78">
+        <v>52212308</v>
+      </c>
+      <c r="M78" t="s">
+        <v>179</v>
+      </c>
+      <c r="N78" t="s">
+        <v>199</v>
+      </c>
+      <c r="O78" t="s">
+        <v>194</v>
+      </c>
+      <c r="P78" t="s">
         <v>195</v>
       </c>
-      <c r="Q77" s="2" t="s">
-        <v>952</v>
-      </c>
-      <c r="R77" s="8">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" ht="34">
-      <c r="A78" s="16">
-        <v>1</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>1070</v>
-      </c>
-      <c r="H78" s="1">
-        <v>1</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>1071</v>
-      </c>
-      <c r="J78" s="1">
-        <v>2020</v>
-      </c>
-      <c r="L78" s="1">
-        <v>46227690</v>
-      </c>
-      <c r="M78" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="N78" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="O78" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P78" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q78" s="2" t="s">
-        <v>621</v>
+      <c r="Q78" s="11" t="s">
+        <v>674</v>
       </c>
       <c r="R78" s="8">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="34">
       <c r="A79" s="17">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>982</v>
+        <v>1087</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>663</v>
+        <v>879</v>
       </c>
       <c r="D79" t="s">
-        <v>662</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>752</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>974</v>
-      </c>
-      <c r="G79">
-        <v>29</v>
-      </c>
-      <c r="H79">
-        <v>2</v>
-      </c>
-      <c r="I79" t="s">
-        <v>1243</v>
+        <v>857</v>
+      </c>
+      <c r="E79" t="s">
+        <v>880</v>
+      </c>
+      <c r="F79" t="s">
+        <v>972</v>
+      </c>
+      <c r="G79" s="1">
+        <v>4</v>
+      </c>
+      <c r="H79" s="1">
+        <v>1</v>
+      </c>
+      <c r="I79" s="1">
+        <v>251524592092800</v>
       </c>
       <c r="J79">
         <v>2020</v>
       </c>
       <c r="K79" t="s">
-        <v>1029</v>
-      </c>
-      <c r="L79">
-        <v>52212308</v>
+        <v>1025</v>
+      </c>
+      <c r="L79" t="s">
+        <v>1089</v>
       </c>
       <c r="M79" t="s">
         <v>179</v>
@@ -8826,72 +8983,72 @@
         <v>199</v>
       </c>
       <c r="O79" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="P79" t="s">
         <v>195</v>
       </c>
       <c r="Q79" s="11" t="s">
-        <v>674</v>
+        <v>881</v>
       </c>
       <c r="R79" s="8">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" ht="34">
-      <c r="A80" s="17">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" ht="51">
+      <c r="A80" s="16">
         <v>1</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1088</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>879</v>
+        <v>1007</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>983</v>
       </c>
       <c r="D80" t="s">
-        <v>857</v>
-      </c>
-      <c r="E80" t="s">
-        <v>880</v>
-      </c>
-      <c r="F80" t="s">
-        <v>973</v>
+        <v>1036</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>1009</v>
       </c>
       <c r="G80" s="1">
+        <v>70</v>
+      </c>
+      <c r="H80" s="1">
         <v>4</v>
       </c>
-      <c r="H80" s="1">
-        <v>1</v>
-      </c>
-      <c r="I80" s="1">
-        <v>251524592092800</v>
-      </c>
-      <c r="J80">
+      <c r="I80" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="J80" s="1">
         <v>2020</v>
       </c>
       <c r="K80" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="L80" t="s">
-        <v>1090</v>
-      </c>
-      <c r="M80" t="s">
+        <v>1049</v>
+      </c>
+      <c r="M80" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="N80" t="s">
-        <v>199</v>
-      </c>
-      <c r="O80" t="s">
-        <v>183</v>
-      </c>
-      <c r="P80" t="s">
+      <c r="N80" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="P80" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q80" s="11" t="s">
-        <v>881</v>
+      <c r="Q80" s="1" t="s">
+        <v>1037</v>
       </c>
       <c r="R80" s="8">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="1:18" ht="51">
@@ -8899,34 +9056,34 @@
         <v>1</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>984</v>
-      </c>
-      <c r="D81" t="s">
-        <v>1037</v>
+        <v>982</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>1034</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="G81" s="1">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="H81" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>1227</v>
+        <v>1054</v>
       </c>
       <c r="J81" s="1">
         <v>2020</v>
       </c>
       <c r="K81" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="L81" t="s">
         <v>1050</v>
@@ -8943,49 +9100,49 @@
       <c r="P81" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q81" s="1" t="s">
-        <v>1038</v>
+      <c r="Q81" s="2" t="s">
+        <v>1035</v>
       </c>
       <c r="R81" s="8">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" ht="51">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" ht="34">
       <c r="A82" s="16">
         <v>1</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1011</v>
+        <v>1093</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>983</v>
+        <v>61</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>1035</v>
+        <v>62</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>1012</v>
+        <v>730</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>1013</v>
+        <v>1081</v>
       </c>
       <c r="G82" s="1">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="H82" s="1">
         <v>5</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>1055</v>
+        <v>1110</v>
       </c>
       <c r="J82" s="1">
-        <v>2020</v>
-      </c>
-      <c r="K82" t="s">
-        <v>1028</v>
-      </c>
-      <c r="L82" t="s">
-        <v>1051</v>
+        <v>2021</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>1111</v>
       </c>
       <c r="M82" s="1" t="s">
         <v>179</v>
@@ -8994,16 +9151,16 @@
         <v>199</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="P82" s="1" t="s">
         <v>195</v>
       </c>
       <c r="Q82" s="2" t="s">
-        <v>1036</v>
+        <v>608</v>
       </c>
       <c r="R82" s="8">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:18" ht="34">
@@ -9013,35 +9170,35 @@
       <c r="B83" s="1" t="s">
         <v>1094</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>62</v>
+      <c r="C83" s="6" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1086</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>730</v>
+        <v>1067</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>1082</v>
+        <v>485</v>
       </c>
       <c r="G83" s="1">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="H83" s="1">
-        <v>5</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>1111</v>
+        <v>3</v>
+      </c>
+      <c r="I83" t="s">
+        <v>1227</v>
       </c>
       <c r="J83" s="1">
         <v>2021</v>
       </c>
-      <c r="K83" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>1112</v>
+      <c r="K83" t="s">
+        <v>1127</v>
+      </c>
+      <c r="L83" t="s">
+        <v>1128</v>
       </c>
       <c r="M83" s="1" t="s">
         <v>179</v>
@@ -9050,54 +9207,51 @@
         <v>199</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="P83" s="1" t="s">
         <v>195</v>
       </c>
       <c r="Q83" s="2" t="s">
-        <v>608</v>
+        <v>1085</v>
       </c>
       <c r="R83" s="8">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:18" ht="34">
       <c r="A84" s="16">
         <v>1</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>1095</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>1127</v>
-      </c>
-      <c r="D84" t="s">
-        <v>1087</v>
+      <c r="B84" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>1107</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>1068</v>
+        <v>988</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>485</v>
+        <v>1073</v>
       </c>
       <c r="G84" s="1">
-        <v>125</v>
+        <v>2</v>
       </c>
       <c r="H84" s="1">
-        <v>3</v>
-      </c>
-      <c r="I84" t="s">
-        <v>1230</v>
+        <v>1</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>1108</v>
       </c>
       <c r="J84" s="1">
         <v>2021</v>
       </c>
       <c r="K84" t="s">
-        <v>1128</v>
-      </c>
-      <c r="L84" t="s">
-        <v>1129</v>
+        <v>1109</v>
+      </c>
+      <c r="L84">
+        <v>92236335</v>
       </c>
       <c r="M84" s="1" t="s">
         <v>179</v>
@@ -9112,45 +9266,45 @@
         <v>195</v>
       </c>
       <c r="Q84" s="2" t="s">
-        <v>1086</v>
+        <v>1140</v>
       </c>
       <c r="R84" s="8">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:18" ht="34">
       <c r="A85" s="16">
         <v>1</v>
       </c>
-      <c r="B85" t="s">
-        <v>1107</v>
+      <c r="B85" s="1" t="s">
+        <v>1219</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1108</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>989</v>
+        <v>1084</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E85" t="s">
+        <v>779</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>1074</v>
+        <v>1082</v>
       </c>
       <c r="G85" s="1">
-        <v>2</v>
-      </c>
-      <c r="H85" s="1">
-        <v>1</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>1109</v>
+        <v>6</v>
+      </c>
+      <c r="I85" s="22" t="s">
+        <v>1220</v>
       </c>
       <c r="J85" s="1">
-        <v>2021</v>
-      </c>
-      <c r="K85" t="s">
-        <v>1110</v>
-      </c>
-      <c r="L85">
-        <v>92236335</v>
+        <v>2022</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>1221</v>
       </c>
       <c r="M85" s="1" t="s">
         <v>179</v>
@@ -9162,48 +9316,42 @@
         <v>194</v>
       </c>
       <c r="P85" s="1" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="Q85" s="2" t="s">
-        <v>1141</v>
-      </c>
-      <c r="R85" s="8">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" ht="34">
+        <v>601</v>
+      </c>
+      <c r="R85">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" ht="68">
       <c r="A86" s="16">
         <v>1</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1222</v>
+        <v>1098</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1085</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E86" t="s">
-        <v>779</v>
+        <v>1095</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>1096</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>1083</v>
-      </c>
-      <c r="G86" s="1">
-        <v>6</v>
-      </c>
-      <c r="I86" s="23" t="s">
-        <v>1223</v>
+        <v>1097</v>
+      </c>
+      <c r="G86">
+        <v>5</v>
+      </c>
+      <c r="I86" s="1">
+        <v>100141</v>
       </c>
       <c r="J86" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>1265</v>
-      </c>
-      <c r="L86" s="1" t="s">
-        <v>1224</v>
+        <v>1105</v>
       </c>
       <c r="M86" s="1" t="s">
         <v>179</v>
@@ -9215,42 +9363,45 @@
         <v>194</v>
       </c>
       <c r="P86" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q86" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="R86">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" ht="68">
+        <v>195</v>
+      </c>
+      <c r="Q86" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="R86" s="8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" ht="34">
       <c r="A87" s="16">
         <v>1</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>1099</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>1096</v>
+        <v>1056</v>
+      </c>
+      <c r="C87" s="23" t="s">
+        <v>1100</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>1097</v>
+        <v>1055</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>1098</v>
-      </c>
-      <c r="G87">
-        <v>5</v>
-      </c>
-      <c r="I87" s="1">
-        <v>100141</v>
+        <v>120</v>
+      </c>
+      <c r="G87" s="1">
+        <v>54</v>
+      </c>
+      <c r="H87" s="1">
+        <v>1</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>1102</v>
       </c>
       <c r="J87" s="1">
-        <v>2021</v>
-      </c>
-      <c r="K87" s="1" t="s">
-        <v>1106</v>
+        <v>2020</v>
+      </c>
+      <c r="K87" t="s">
+        <v>1233</v>
       </c>
       <c r="M87" s="1" t="s">
         <v>179</v>
@@ -9259,16 +9410,16 @@
         <v>199</v>
       </c>
       <c r="O87" s="1" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="P87" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q87" s="1" t="s">
-        <v>1100</v>
+      <c r="Q87" s="2" t="s">
+        <v>1139</v>
       </c>
       <c r="R87" s="8">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="88" spans="1:18" ht="34">
@@ -9276,13 +9427,13 @@
         <v>1</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1057</v>
-      </c>
-      <c r="C88" s="24" t="s">
-        <v>1101</v>
+        <v>1133</v>
+      </c>
+      <c r="C88" s="25" t="s">
+        <v>1061</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>1056</v>
+        <v>1062</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>120</v>
@@ -9291,16 +9442,16 @@
         <v>54</v>
       </c>
       <c r="H88" s="1">
-        <v>1</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>1103</v>
+        <v>4</v>
+      </c>
+      <c r="I88" t="s">
+        <v>1260</v>
       </c>
       <c r="J88" s="1">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="K88" t="s">
-        <v>1236</v>
+        <v>1119</v>
       </c>
       <c r="M88" s="1" t="s">
         <v>179</v>
@@ -9309,48 +9460,51 @@
         <v>199</v>
       </c>
       <c r="O88" s="1" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="P88" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q88" s="2" t="s">
-        <v>1140</v>
+        <v>185</v>
+      </c>
+      <c r="Q88" s="11" t="s">
+        <v>1134</v>
       </c>
       <c r="R88" s="8">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" ht="34">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" ht="17">
       <c r="A89" s="16">
         <v>1</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>1134</v>
-      </c>
-      <c r="C89" s="26" t="s">
-        <v>1062</v>
+      <c r="B89" s="2" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="D89" s="20" t="s">
+        <v>967</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>1063</v>
+        <v>969</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G89" s="1">
-        <v>54</v>
-      </c>
-      <c r="H89" s="1">
-        <v>4</v>
-      </c>
-      <c r="I89" t="s">
-        <v>1264</v>
+        <v>1197</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I89" s="1">
+        <v>1274</v>
       </c>
       <c r="J89" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="K89" t="s">
-        <v>1120</v>
+        <v>970</v>
+      </c>
+      <c r="L89">
+        <v>66565618</v>
       </c>
       <c r="M89" s="1" t="s">
         <v>179</v>
@@ -9362,48 +9516,39 @@
         <v>194</v>
       </c>
       <c r="P89" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q89" s="11" t="s">
-        <v>1135</v>
+        <v>195</v>
+      </c>
+      <c r="Q89" s="2" t="s">
+        <v>971</v>
       </c>
       <c r="R89" s="8">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" ht="17">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" ht="34">
       <c r="A90" s="16">
         <v>1</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>1199</v>
-      </c>
       <c r="C90" s="1" t="s">
-        <v>969</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>968</v>
+        <v>1030</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>970</v>
+        <v>1031</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>1200</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>1198</v>
+        <v>1032</v>
+      </c>
+      <c r="G90">
+        <v>100</v>
       </c>
       <c r="I90" s="1">
-        <v>1274</v>
+        <v>104280</v>
       </c>
       <c r="J90" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="K90" t="s">
-        <v>971</v>
-      </c>
-      <c r="L90">
-        <v>66565618</v>
+        <v>1214</v>
       </c>
       <c r="M90" s="1" t="s">
         <v>179</v>
@@ -9418,36 +9563,48 @@
         <v>195</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>972</v>
+        <v>1138</v>
       </c>
       <c r="R90" s="8">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="1:18" ht="34">
       <c r="A91" s="16">
         <v>1</v>
       </c>
+      <c r="B91" s="1" t="s">
+        <v>1198</v>
+      </c>
       <c r="C91" s="1" t="s">
-        <v>1031</v>
+        <v>1101</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>1047</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>1032</v>
+        <v>1048</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1033</v>
+        <v>75</v>
       </c>
       <c r="G91">
-        <v>100</v>
-      </c>
-      <c r="I91" s="1">
-        <v>104280</v>
+        <v>5</v>
+      </c>
+      <c r="H91" s="1">
+        <v>8</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>1103</v>
       </c>
       <c r="J91" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K91" t="s">
-        <v>1217</v>
+        <v>2021</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="L91">
+        <v>93001247</v>
       </c>
       <c r="M91" s="1" t="s">
         <v>179</v>
@@ -9456,54 +9613,51 @@
         <v>199</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="P91" s="1" t="s">
         <v>195</v>
       </c>
       <c r="Q91" s="2" t="s">
-        <v>1139</v>
+        <v>1046</v>
       </c>
       <c r="R91" s="8">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" ht="34">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="51">
       <c r="A92" s="16">
         <v>1</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" t="s">
         <v>1201</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1102</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>1048</v>
+        <v>993</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>1049</v>
+        <v>1202</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G92">
-        <v>5</v>
+        <v>1072</v>
+      </c>
+      <c r="G92" s="1">
+        <v>53</v>
       </c>
       <c r="H92" s="1">
-        <v>8</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>1104</v>
+        <v>3</v>
+      </c>
+      <c r="I92" t="s">
+        <v>1239</v>
       </c>
       <c r="J92" s="1">
-        <v>2021</v>
-      </c>
-      <c r="K92" s="1" t="s">
-        <v>1105</v>
+        <v>2022</v>
+      </c>
+      <c r="K92" t="s">
+        <v>1203</v>
       </c>
       <c r="L92">
-        <v>93001247</v>
+        <v>110569695</v>
       </c>
       <c r="M92" s="1" t="s">
         <v>179</v>
@@ -9512,16 +9666,16 @@
         <v>199</v>
       </c>
       <c r="O92" s="1" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="P92" s="1" t="s">
         <v>195</v>
       </c>
       <c r="Q92" s="2" t="s">
-        <v>1047</v>
+        <v>1141</v>
       </c>
       <c r="R92" s="8">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:18" ht="51">
@@ -9529,34 +9683,34 @@
         <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>994</v>
+        <v>1242</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>1042</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>1205</v>
+        <v>1043</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>1073</v>
+        <v>75</v>
       </c>
       <c r="G93" s="1">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="H93" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I93" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="J93" s="1">
         <v>2022</v>
       </c>
       <c r="K93" t="s">
-        <v>1206</v>
-      </c>
-      <c r="L93">
-        <v>110569695</v>
+        <v>1311</v>
       </c>
       <c r="M93" s="1" t="s">
         <v>179</v>
@@ -9565,16 +9719,16 @@
         <v>199</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="P93" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q93" s="2" t="s">
-        <v>1142</v>
-      </c>
-      <c r="R93" s="8">
-        <v>71</v>
+      <c r="Q93" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="R93" s="1">
+        <v>72</v>
       </c>
     </row>
     <row r="94" spans="1:18" ht="51">
@@ -9582,34 +9736,37 @@
         <v>1</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>1245</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>1221</v>
+        <v>1231</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>960</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>1043</v>
+        <v>19</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>1044</v>
+        <v>1199</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>75</v>
+        <v>1200</v>
       </c>
       <c r="G94" s="1">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="H94" s="1">
-        <v>6</v>
-      </c>
-      <c r="I94" t="s">
-        <v>1244</v>
+        <v>1</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>1232</v>
       </c>
       <c r="J94" s="1">
         <v>2022</v>
       </c>
-      <c r="K94" t="s">
-        <v>1260</v>
+      <c r="K94" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="L94" s="1">
+        <v>46227693</v>
       </c>
       <c r="M94" s="1" t="s">
         <v>179</v>
@@ -9618,16 +9775,16 @@
         <v>199</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="P94" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q94" s="1" t="s">
-        <v>1046</v>
+        <v>185</v>
+      </c>
+      <c r="Q94" s="2" t="s">
+        <v>458</v>
       </c>
       <c r="R94" s="1">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:18" ht="51">
@@ -9635,37 +9792,37 @@
         <v>1</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>1234</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>961</v>
+        <v>1301</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>1259</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>19</v>
+        <v>1124</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>1202</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>1203</v>
-      </c>
-      <c r="G95" s="1">
-        <v>26</v>
-      </c>
-      <c r="H95" s="1">
-        <v>1</v>
+        <v>1125</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>1083</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>1235</v>
+        <v>274</v>
       </c>
       <c r="J95" s="1">
         <v>2022</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>1233</v>
-      </c>
-      <c r="L95" s="1">
-        <v>46227693</v>
+        <v>1206</v>
+      </c>
+      <c r="L95" s="1" t="s">
+        <v>1303</v>
       </c>
       <c r="M95" s="1" t="s">
         <v>179</v>
@@ -9677,42 +9834,48 @@
         <v>194</v>
       </c>
       <c r="P95" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q95" s="2" t="s">
-        <v>458</v>
+        <v>195</v>
+      </c>
+      <c r="Q95" s="1" t="s">
+        <v>1147</v>
       </c>
       <c r="R95" s="1">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="96" spans="1:18" ht="34">
       <c r="A96" s="16">
         <v>1</v>
       </c>
-      <c r="C96" s="24" t="s">
-        <v>830</v>
+      <c r="B96" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>1153</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>207</v>
+        <v>1155</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>178</v>
+        <v>1205</v>
+      </c>
+      <c r="G96" s="1">
+        <v>119</v>
+      </c>
+      <c r="H96" s="1">
+        <v>22</v>
+      </c>
+      <c r="I96" t="s">
+        <v>1229</v>
       </c>
       <c r="J96" s="1">
-        <v>2008</v>
+        <v>2022</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>41</v>
+        <v>1228</v>
       </c>
       <c r="M96" s="1" t="s">
         <v>179</v>
@@ -9721,16 +9884,16 @@
         <v>199</v>
       </c>
       <c r="O96" s="1" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="P96" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q96" s="11" t="s">
-        <v>565</v>
-      </c>
-      <c r="R96" s="8" t="s">
-        <v>946</v>
+        <v>195</v>
+      </c>
+      <c r="Q96" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="R96" s="1">
+        <v>75</v>
       </c>
     </row>
     <row r="97" spans="1:18" ht="34">
@@ -9738,16 +9901,16 @@
         <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>1114</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>1116</v>
-      </c>
       <c r="F97" s="1" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>178</v>
@@ -9762,7 +9925,7 @@
         <v>2022</v>
       </c>
       <c r="K97" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="L97">
         <v>93463381</v>
@@ -9780,24 +9943,24 @@
         <v>195</v>
       </c>
       <c r="Q97" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="R97" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="1:18" ht="17">
+    <row r="98" spans="1:18" ht="34">
       <c r="A98" s="16">
         <v>1</v>
       </c>
-      <c r="C98" t="s">
-        <v>1237</v>
+      <c r="C98" s="6" t="s">
+        <v>1234</v>
       </c>
       <c r="D98" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E98" s="1" t="s">
         <v>1118</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>1119</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>75</v>
@@ -9806,16 +9969,16 @@
         <v>2021</v>
       </c>
       <c r="K98" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
       <c r="L98" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="M98" s="1" t="s">
         <v>179</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="O98" s="1" t="s">
         <v>194</v>
@@ -9824,31 +9987,40 @@
         <v>185</v>
       </c>
       <c r="Q98" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="R98" s="1"/>
     </row>
-    <row r="99" spans="1:18" ht="34">
+    <row r="99" spans="1:18" ht="51">
       <c r="A99" s="16">
         <v>1</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>928</v>
-      </c>
-      <c r="C99" s="24" t="s">
-        <v>927</v>
+      <c r="C99" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>1150</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>929</v>
+        <v>1154</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>930</v>
+        <v>1226</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>1309</v>
       </c>
       <c r="J99" s="1">
-        <v>2016</v>
-      </c>
-      <c r="L99">
-        <v>46227876</v>
+        <v>2022</v>
+      </c>
+      <c r="K99" t="s">
+        <v>1310</v>
       </c>
       <c r="M99" s="1" t="s">
         <v>179</v>
@@ -9862,25 +10034,25 @@
       <c r="P99" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q99" s="2" t="s">
-        <v>629</v>
-      </c>
-      <c r="R99" s="8" t="s">
-        <v>946</v>
+      <c r="Q99" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="R99" s="1">
+        <v>77</v>
       </c>
     </row>
     <row r="100" spans="1:18" ht="34">
       <c r="A100" s="16">
         <v>1</v>
       </c>
-      <c r="C100" s="26" t="s">
+      <c r="C100" s="25" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E100" s="1" t="s">
         <v>1121</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="F100" s="1" t="s">
         <v>1122</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>1123</v>
       </c>
       <c r="J100" s="1">
         <v>2021</v>
@@ -9899,7 +10071,7 @@
         <v>185</v>
       </c>
       <c r="Q100" s="11" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="R100" s="1"/>
     </row>
@@ -9907,35 +10079,32 @@
       <c r="A101" s="16">
         <v>1</v>
       </c>
-      <c r="C101" s="6" t="s">
-        <v>1263</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>1125</v>
+      <c r="B101" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C101" s="26" t="s">
+        <v>1243</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>1126</v>
-      </c>
-      <c r="F101" t="s">
-        <v>1207</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H101" s="1" t="s">
-        <v>1084</v>
+        <v>1245</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G101" s="1">
+        <v>7</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>274</v>
+        <v>1302</v>
       </c>
       <c r="J101" s="1">
         <v>2022</v>
       </c>
-      <c r="K101" s="1" t="s">
-        <v>1209</v>
-      </c>
-      <c r="L101" s="1">
-        <v>101888659</v>
+      <c r="K101" t="s">
+        <v>1254</v>
+      </c>
+      <c r="L101">
+        <v>118314400</v>
       </c>
       <c r="M101" s="1" t="s">
         <v>179</v>
@@ -9949,31 +10118,43 @@
       <c r="P101" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q101" s="1" t="s">
+      <c r="Q101" s="2" t="s">
+        <v>1248</v>
+      </c>
+      <c r="R101" s="8">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" ht="51">
+      <c r="A102" s="16">
+        <v>1</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>1148</v>
       </c>
-      <c r="R101" s="1">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" ht="68">
-      <c r="A102" s="16">
-        <v>1</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>1149</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>1150</v>
+      <c r="F102" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>274</v>
       </c>
       <c r="J102" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="M102" s="1" t="s">
         <v>179</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O102" s="1" t="s">
         <v>194</v>
@@ -9981,39 +10162,41 @@
       <c r="P102" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q102" s="1" t="s">
-        <v>946</v>
-      </c>
-      <c r="R102" s="1"/>
-    </row>
-    <row r="103" spans="1:18" ht="51">
+      <c r="Q102" s="2" t="s">
+        <v>1266</v>
+      </c>
+      <c r="R102" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" ht="34">
       <c r="A103" s="16">
         <v>1</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>1152</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>1153</v>
+      <c r="B103" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C103" s="26" t="s">
+        <v>1249</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>1157</v>
+        <v>1250</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>1229</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H103" s="1" t="s">
-        <v>178</v>
+        <v>1251</v>
+      </c>
+      <c r="G103" s="1">
+        <v>26</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>274</v>
+        <v>1300</v>
       </c>
       <c r="J103" s="1">
         <v>2022</v>
       </c>
+      <c r="K103" t="s">
+        <v>1255</v>
+      </c>
       <c r="M103" s="1" t="s">
         <v>179</v>
       </c>
@@ -10026,11 +10209,11 @@
       <c r="P103" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q103" s="1" t="s">
-        <v>1151</v>
-      </c>
-      <c r="R103" s="1">
-        <v>77</v>
+      <c r="Q103" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="R103" s="8">
+        <v>79</v>
       </c>
     </row>
     <row r="104" spans="1:18" ht="34">
@@ -10038,34 +10221,37 @@
         <v>1</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>1228</v>
+        <v>1262</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1155</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>1156</v>
+        <v>953</v>
+      </c>
+      <c r="D104" t="s">
+        <v>954</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>1158</v>
+        <v>955</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>1208</v>
-      </c>
-      <c r="G104" s="1">
-        <v>119</v>
-      </c>
-      <c r="H104" s="1">
-        <v>22</v>
-      </c>
-      <c r="I104" t="s">
-        <v>1232</v>
+        <v>1263</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>1264</v>
       </c>
       <c r="J104" s="1">
         <v>2022</v>
       </c>
-      <c r="K104" s="1" t="s">
-        <v>1231</v>
+      <c r="K104" t="s">
+        <v>966</v>
+      </c>
+      <c r="L104">
+        <v>66133660</v>
       </c>
       <c r="M104" s="1" t="s">
         <v>179</v>
@@ -10079,11 +10265,11 @@
       <c r="P104" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Q104" s="1" t="s">
-        <v>1154</v>
+      <c r="Q104" s="11" t="s">
+        <v>956</v>
       </c>
       <c r="R104" s="1">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:18" ht="34">
@@ -11414,7 +11600,7 @@
         <v>299</v>
       </c>
       <c r="K142" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="L142" s="1"/>
       <c r="M142" s="1" t="s">
@@ -11935,7 +12121,7 @@
         <v>760</v>
       </c>
       <c r="F155" s="6" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
@@ -13245,7 +13431,7 @@
         <v>195</v>
       </c>
       <c r="Q193" s="2" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="R193" s="1"/>
     </row>
@@ -13507,7 +13693,7 @@
       </c>
       <c r="B201"/>
       <c r="C201" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D201"/>
       <c r="E201" s="1" t="s">
@@ -13634,7 +13820,7 @@
         <v>810</v>
       </c>
       <c r="F204" s="6" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="G204"/>
       <c r="H204"/>
@@ -13643,7 +13829,7 @@
         <v>811</v>
       </c>
       <c r="K204" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="L204"/>
       <c r="M204" s="1" t="s">
@@ -13677,7 +13863,7 @@
         <v>852</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="J205" s="1" t="s">
         <v>811</v>
@@ -13888,7 +14074,7 @@
         <v>195</v>
       </c>
       <c r="Q210" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="R210" s="1"/>
     </row>
@@ -13896,7 +14082,7 @@
       <c r="A211" s="16">
         <v>1</v>
       </c>
-      <c r="C211" s="20" t="s">
+      <c r="C211" s="19" t="s">
         <v>904</v>
       </c>
       <c r="E211" s="1" t="s">
@@ -13930,7 +14116,7 @@
         <v>1</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>871</v>
@@ -14038,16 +14224,16 @@
         <v>1</v>
       </c>
       <c r="C215" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="F215" s="1" t="s">
         <v>986</v>
       </c>
-      <c r="E215" s="1" t="s">
-        <v>985</v>
-      </c>
-      <c r="F215" s="1" t="s">
+      <c r="J215" s="1" t="s">
         <v>987</v>
-      </c>
-      <c r="J215" s="1" t="s">
-        <v>988</v>
       </c>
       <c r="M215" s="1" t="s">
         <v>215</v>
@@ -14062,7 +14248,7 @@
         <v>195</v>
       </c>
       <c r="Q215" s="2" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="R215" s="1"/>
     </row>
@@ -14071,16 +14257,16 @@
         <v>1</v>
       </c>
       <c r="C216" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="E216" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="E216" s="1" t="s">
-        <v>996</v>
-      </c>
       <c r="F216" s="1" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="J216" s="1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="M216" s="1" t="s">
         <v>215</v>
@@ -14095,7 +14281,7 @@
         <v>195</v>
       </c>
       <c r="Q216" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="R216" s="1"/>
     </row>
@@ -14104,16 +14290,16 @@
         <v>1</v>
       </c>
       <c r="C217" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="E217" s="1" t="s">
         <v>997</v>
       </c>
-      <c r="E217" s="1" t="s">
-        <v>998</v>
-      </c>
       <c r="F217" s="1" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="J217" s="1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="M217" s="1" t="s">
         <v>215</v>
@@ -14128,7 +14314,7 @@
         <v>195</v>
       </c>
       <c r="Q217" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="R217" s="1"/>
     </row>
@@ -14137,16 +14323,16 @@
         <v>1</v>
       </c>
       <c r="C218" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="E218" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="E218" s="1" t="s">
-        <v>1000</v>
-      </c>
       <c r="F218" s="1" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="J218" s="1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="M218" s="1" t="s">
         <v>215</v>
@@ -14161,7 +14347,7 @@
         <v>195</v>
       </c>
       <c r="Q218" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="R218" s="1"/>
     </row>
@@ -14170,16 +14356,16 @@
         <v>1</v>
       </c>
       <c r="C219" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E219" s="1" t="s">
         <v>1001</v>
       </c>
-      <c r="E219" s="1" t="s">
+      <c r="F219" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="J219" s="1" t="s">
         <v>1002</v>
-      </c>
-      <c r="F219" s="1" t="s">
-        <v>1018</v>
-      </c>
-      <c r="J219" s="1" t="s">
-        <v>1003</v>
       </c>
       <c r="M219" s="1" t="s">
         <v>215</v>
@@ -14194,7 +14380,7 @@
         <v>195</v>
       </c>
       <c r="Q219" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="R219" s="1"/>
     </row>
@@ -14203,16 +14389,16 @@
         <v>1</v>
       </c>
       <c r="C220" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="F220" s="1" t="s">
         <v>990</v>
       </c>
-      <c r="E220" s="1" t="s">
-        <v>989</v>
-      </c>
-      <c r="F220" s="1" t="s">
+      <c r="J220" s="1" t="s">
         <v>991</v>
-      </c>
-      <c r="J220" s="1" t="s">
-        <v>992</v>
       </c>
       <c r="M220" s="1" t="s">
         <v>215</v>
@@ -14227,7 +14413,7 @@
         <v>195</v>
       </c>
       <c r="Q220" s="2" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="R220" s="1"/>
     </row>
@@ -14236,16 +14422,16 @@
         <v>1</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="J221" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="M221" s="1" t="s">
         <v>215</v>
@@ -14260,7 +14446,7 @@
         <v>195</v>
       </c>
       <c r="Q221" s="2" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="R221" s="1"/>
     </row>
@@ -14269,16 +14455,16 @@
         <v>1</v>
       </c>
       <c r="C222" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E222" s="1" t="s">
         <v>1014</v>
       </c>
-      <c r="E222" s="1" t="s">
+      <c r="F222" s="1" t="s">
         <v>1015</v>
       </c>
-      <c r="F222" s="1" t="s">
-        <v>1016</v>
-      </c>
       <c r="J222" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="M222" s="1" t="s">
         <v>215</v>
@@ -14293,7 +14479,7 @@
         <v>185</v>
       </c>
       <c r="Q222" s="11" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="R222" s="1"/>
     </row>
@@ -14302,16 +14488,16 @@
         <v>1</v>
       </c>
       <c r="C223" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E223" s="1" t="s">
         <v>1019</v>
       </c>
-      <c r="E223" s="1" t="s">
+      <c r="F223" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="F223" s="1" t="s">
-        <v>1021</v>
-      </c>
       <c r="J223" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="M223" s="1" t="s">
         <v>215</v>
@@ -14326,7 +14512,7 @@
         <v>185</v>
       </c>
       <c r="Q223" s="11" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="R223" s="1"/>
     </row>
@@ -14335,16 +14521,16 @@
         <v>1</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="J224" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="M224" s="1" t="s">
         <v>215</v>
@@ -14359,7 +14545,7 @@
         <v>185</v>
       </c>
       <c r="Q224" s="11" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="R224" s="1"/>
     </row>
@@ -14367,17 +14553,17 @@
       <c r="A225" s="16">
         <v>1</v>
       </c>
-      <c r="C225" s="26" t="s">
+      <c r="C225" s="25" t="s">
+        <v>1061</v>
+      </c>
+      <c r="E225" s="1" t="s">
         <v>1062</v>
       </c>
-      <c r="E225" s="1" t="s">
-        <v>1063</v>
-      </c>
       <c r="F225" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="J225" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="M225" s="1" t="s">
         <v>215</v>
@@ -14392,7 +14578,7 @@
         <v>185</v>
       </c>
       <c r="Q225" s="11" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="R225" s="1"/>
     </row>
@@ -14401,16 +14587,16 @@
         <v>1</v>
       </c>
       <c r="C226" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E226" s="1" t="s">
         <v>1064</v>
       </c>
-      <c r="E226" s="1" t="s">
+      <c r="F226" s="1" t="s">
         <v>1065</v>
       </c>
-      <c r="F226" s="1" t="s">
-        <v>1066</v>
-      </c>
       <c r="J226" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="M226" s="1" t="s">
         <v>215</v>
@@ -14424,8 +14610,8 @@
       <c r="P226" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="Q226" s="23" t="s">
-        <v>1067</v>
+      <c r="Q226" s="22" t="s">
+        <v>1066</v>
       </c>
       <c r="R226" s="1"/>
     </row>
@@ -14434,16 +14620,16 @@
         <v>1</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="J227" s="1" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="M227" s="1" t="s">
         <v>215</v>
@@ -14458,7 +14644,7 @@
         <v>185</v>
       </c>
       <c r="Q227" s="2" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
       <c r="R227" s="1"/>
     </row>
@@ -14467,16 +14653,16 @@
         <v>1</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
       <c r="J228" s="1" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="M228" s="1" t="s">
         <v>215</v>
@@ -14491,7 +14677,7 @@
         <v>195</v>
       </c>
       <c r="Q228" s="2" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="R228" s="1"/>
     </row>
@@ -14500,16 +14686,16 @@
         <v>1</v>
       </c>
       <c r="C229" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E229" s="1" t="s">
         <v>1076</v>
       </c>
-      <c r="E229" s="1" t="s">
-        <v>1077</v>
-      </c>
       <c r="F229" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="J229" s="1" t="s">
         <v>1080</v>
-      </c>
-      <c r="J229" s="1" t="s">
-        <v>1081</v>
       </c>
       <c r="M229" s="1" t="s">
         <v>215</v>
@@ -14533,16 +14719,16 @@
         <v>1</v>
       </c>
       <c r="C230" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E230" s="1" t="s">
         <v>1078</v>
       </c>
-      <c r="E230" s="1" t="s">
+      <c r="F230" s="1" t="s">
         <v>1079</v>
       </c>
-      <c r="F230" s="1" t="s">
+      <c r="J230" s="1" t="s">
         <v>1080</v>
-      </c>
-      <c r="J230" s="1" t="s">
-        <v>1081</v>
       </c>
       <c r="M230" s="1" t="s">
         <v>215</v>
@@ -14566,16 +14752,16 @@
         <v>1</v>
       </c>
       <c r="C231" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="J231" s="1" t="s">
         <v>1159</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>1160</v>
-      </c>
-      <c r="F231" s="1" t="s">
-        <v>1161</v>
-      </c>
-      <c r="J231" s="1" t="s">
-        <v>1162</v>
       </c>
       <c r="M231" s="1" t="s">
         <v>215</v>
@@ -14590,7 +14776,7 @@
         <v>195</v>
       </c>
       <c r="Q231" s="2" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="R231" s="1"/>
     </row>
@@ -14599,16 +14785,16 @@
         <v>1</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>385</v>
       </c>
       <c r="J232" s="1" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="M232" s="1" t="s">
         <v>215</v>
@@ -14623,7 +14809,7 @@
         <v>195</v>
       </c>
       <c r="Q232" s="2" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="R232" s="1"/>
     </row>
@@ -14632,16 +14818,16 @@
         <v>1</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="J233" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="M233" s="1" t="s">
         <v>215</v>
@@ -14656,7 +14842,7 @@
         <v>195</v>
       </c>
       <c r="Q233" s="2" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="R233" s="1"/>
     </row>
@@ -14665,16 +14851,16 @@
         <v>1</v>
       </c>
       <c r="C234" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F234" s="1" t="s">
         <v>1184</v>
       </c>
-      <c r="E234" s="1" t="s">
-        <v>1185</v>
-      </c>
-      <c r="F234" s="1" t="s">
-        <v>1187</v>
-      </c>
       <c r="J234" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="M234" s="1" t="s">
         <v>215</v>
@@ -14689,7 +14875,7 @@
         <v>185</v>
       </c>
       <c r="Q234" s="2" t="s">
-        <v>1186</v>
+        <v>1183</v>
       </c>
       <c r="R234" s="1"/>
     </row>
@@ -14698,16 +14884,16 @@
         <v>1</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="E235" s="1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F235" s="3" t="s">
         <v>1185</v>
       </c>
-      <c r="F235" s="3" t="s">
-        <v>1188</v>
-      </c>
       <c r="J235" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="M235" s="1" t="s">
         <v>215</v>
@@ -14722,7 +14908,7 @@
         <v>185</v>
       </c>
       <c r="Q235" s="2" t="s">
-        <v>1190</v>
+        <v>1187</v>
       </c>
       <c r="R235" s="1"/>
     </row>
@@ -14731,16 +14917,16 @@
         <v>1</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="F236" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J236" s="1" t="s">
         <v>1174</v>
-      </c>
-      <c r="J236" s="1" t="s">
-        <v>1177</v>
       </c>
       <c r="M236" s="1" t="s">
         <v>215</v>
@@ -14755,7 +14941,7 @@
         <v>195</v>
       </c>
       <c r="Q236" s="2" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="R236" s="1"/>
     </row>
@@ -14764,16 +14950,16 @@
         <v>1</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="F237" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J237" s="1" t="s">
         <v>1174</v>
-      </c>
-      <c r="J237" s="1" t="s">
-        <v>1177</v>
       </c>
       <c r="M237" s="1" t="s">
         <v>215</v>
@@ -14788,7 +14974,7 @@
         <v>185</v>
       </c>
       <c r="Q237" s="2" t="s">
-        <v>1181</v>
+        <v>1178</v>
       </c>
       <c r="R237" s="1"/>
     </row>
@@ -14797,16 +14983,16 @@
         <v>1</v>
       </c>
       <c r="C238" s="1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F238" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="J238" s="1" t="s">
         <v>1191</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>1195</v>
-      </c>
-      <c r="F238" s="1" t="s">
-        <v>1193</v>
-      </c>
-      <c r="J238" s="1" t="s">
-        <v>1194</v>
       </c>
       <c r="M238" s="1" t="s">
         <v>215</v>
@@ -14830,16 +15016,16 @@
         <v>1</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>1196</v>
+        <v>1193</v>
       </c>
       <c r="F239" s="1" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
       <c r="J239" s="1" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="M239" s="1" t="s">
         <v>215</v>
@@ -14866,7 +15052,7 @@
         <v>349</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="E240" s="7" t="s">
         <v>734</v>
@@ -14876,7 +15062,7 @@
         <v>2022</v>
       </c>
       <c r="K240" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="L240">
         <v>105725802</v>
@@ -14894,7 +15080,7 @@
         <v>195</v>
       </c>
       <c r="Q240" s="2" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="R240" s="1"/>
     </row>
@@ -14902,17 +15088,17 @@
       <c r="A241">
         <v>1</v>
       </c>
-      <c r="C241" t="s">
-        <v>1218</v>
+      <c r="C241" s="6" t="s">
+        <v>1215</v>
       </c>
       <c r="E241" s="6" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="J241">
         <v>2022</v>
       </c>
       <c r="K241" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="M241" s="1" t="s">
         <v>179</v>
@@ -14935,10 +15121,10 @@
         <v>1</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="J242" s="1">
         <v>2022</v>
@@ -14964,19 +15150,31 @@
         <v>1</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>1185</v>
+        <v>1182</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="G243" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H243" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I243" s="1" t="s">
+        <v>274</v>
       </c>
       <c r="J243" s="1">
         <v>2022</v>
       </c>
       <c r="K243" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="L243">
         <v>113656926</v>
@@ -14985,7 +15183,7 @@
         <v>179</v>
       </c>
       <c r="N243" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O243" s="1" t="s">
         <v>194</v>
@@ -14994,24 +15192,24 @@
         <v>195</v>
       </c>
       <c r="Q243" s="2" t="s">
-        <v>1241</v>
-      </c>
-    </row>
-    <row r="244" spans="1:18" ht="51">
+        <v>1238</v>
+      </c>
+      <c r="R243" s="8">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="244" spans="1:18" ht="34">
       <c r="A244" s="16">
         <v>1</v>
       </c>
-      <c r="B244" s="1" t="s">
-        <v>1247</v>
-      </c>
-      <c r="C244" s="27" t="s">
-        <v>1246</v>
+      <c r="C244" s="23" t="s">
+        <v>830</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>1248</v>
+        <v>207</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>1249</v>
+        <v>566</v>
       </c>
       <c r="G244" s="1" t="s">
         <v>178</v>
@@ -15020,16 +15218,13 @@
         <v>178</v>
       </c>
       <c r="I244" s="1" t="s">
-        <v>274</v>
+        <v>178</v>
       </c>
       <c r="J244" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K244" t="s">
-        <v>1257</v>
-      </c>
-      <c r="L244">
-        <v>118314400</v>
+        <v>2008</v>
+      </c>
+      <c r="K244" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="M244" s="1" t="s">
         <v>179</v>
@@ -15038,16 +15233,16 @@
         <v>199</v>
       </c>
       <c r="O244" s="1" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="P244" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q244" s="2" t="s">
-        <v>1251</v>
-      </c>
-      <c r="R244" s="8">
-        <v>78</v>
+        <v>185</v>
+      </c>
+      <c r="Q244" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="R244" s="8" t="s">
+        <v>946</v>
       </c>
     </row>
     <row r="245" spans="1:18" ht="34">
@@ -15055,31 +15250,22 @@
         <v>1</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>1256</v>
-      </c>
-      <c r="C245" s="27" t="s">
-        <v>1252</v>
+        <v>928</v>
+      </c>
+      <c r="C245" s="23" t="s">
+        <v>927</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>1253</v>
+        <v>929</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>1254</v>
-      </c>
-      <c r="G245" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H245" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="I245" s="1" t="s">
-        <v>274</v>
+        <v>930</v>
       </c>
       <c r="J245" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K245" t="s">
-        <v>1258</v>
+        <v>2016</v>
+      </c>
+      <c r="L245">
+        <v>46227876</v>
       </c>
       <c r="M245" s="1" t="s">
         <v>179</v>
@@ -15094,34 +15280,366 @@
         <v>195</v>
       </c>
       <c r="Q245" s="2" t="s">
-        <v>1255</v>
-      </c>
-      <c r="R245" s="8">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="246" spans="1:18">
-      <c r="C246" s="11"/>
-    </row>
-    <row r="247" spans="1:18">
-      <c r="C247" s="11"/>
-    </row>
-    <row r="248" spans="1:18">
-      <c r="C248" s="11"/>
-    </row>
-    <row r="249" spans="1:18">
-      <c r="C249" s="11"/>
-    </row>
-    <row r="250" spans="1:18">
-      <c r="C250" s="11"/>
-    </row>
-    <row r="251" spans="1:18">
-      <c r="C251" s="11"/>
-    </row>
-    <row r="252" spans="1:18">
-      <c r="C252" s="11"/>
+        <v>629</v>
+      </c>
+      <c r="R245" s="8" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="246" spans="1:18" ht="51">
+      <c r="A246" s="16">
+        <v>1</v>
+      </c>
+      <c r="C246" s="29" t="s">
+        <v>1267</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="J246" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="M246" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N246" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O246" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="P246" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q246" s="1" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="247" spans="1:18" ht="51">
+      <c r="A247" s="16">
+        <v>1</v>
+      </c>
+      <c r="C247" s="28" t="s">
+        <v>1272</v>
+      </c>
+      <c r="E247" s="30" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>1273</v>
+      </c>
+      <c r="J247" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="M247" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N247" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O247" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P247" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q247" s="1" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="248" spans="1:18" ht="34">
+      <c r="A248" s="16">
+        <v>1</v>
+      </c>
+      <c r="C248" s="28" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E248" s="30" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="J248" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="M248" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N248" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O248" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P248" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q248" s="1" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="249" spans="1:18" ht="51">
+      <c r="A249" s="16">
+        <v>1</v>
+      </c>
+      <c r="C249" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E249" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="J249" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="M249" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N249" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O249" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P249" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q249" s="2" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="250" spans="1:18" ht="34">
+      <c r="A250" s="16">
+        <v>1</v>
+      </c>
+      <c r="C250" s="28" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E250" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="J250" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="M250" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N250" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O250" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P250" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q250" s="2" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="251" spans="1:18" ht="34">
+      <c r="A251" s="16">
+        <v>1</v>
+      </c>
+      <c r="C251" s="28" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>1285</v>
+      </c>
+      <c r="J251" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="M251" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N251" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O251" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P251" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q251" s="1" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="252" spans="1:18" ht="34">
+      <c r="A252" s="16">
+        <v>1</v>
+      </c>
+      <c r="C252" s="28" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="J252" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="M252" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N252" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O252" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P252" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q252" s="2" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="253" spans="1:18" ht="34">
+      <c r="A253" s="16">
+        <v>1</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="J253" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="M253" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N253" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O253" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P253" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q253" s="1" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="254" spans="1:18" ht="51">
+      <c r="A254" s="16">
+        <v>1</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>1292</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>1293</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>1294</v>
+      </c>
+      <c r="J254" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="M254" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N254" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O254" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P254" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q254" s="2" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="255" spans="1:18" ht="34">
+      <c r="A255" s="16">
+        <v>1</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="J255" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="M255" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N255" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O255" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P255" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q255" s="2" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="256" spans="1:18" ht="68">
+      <c r="A256" s="16">
+        <v>1</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="J256" s="1">
+        <v>2022</v>
+      </c>
+      <c r="K256" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="M256" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N256" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O256" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P256" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q256" s="1" t="s">
+        <v>1307</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R256" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R239">
     <sortCondition ref="J2:J239"/>
   </sortState>
@@ -15140,7 +15658,7 @@
     <hyperlink ref="Q58" r:id="rId3" xr:uid="{87AB72C3-9098-A544-927E-E80711BFAFD4}"/>
     <hyperlink ref="Q32" r:id="rId4" xr:uid="{36FFD1D9-7B90-594C-A2F7-42E8D063CAE6}"/>
     <hyperlink ref="Q35" r:id="rId5" xr:uid="{662F4851-B5BC-C148-A8A4-D3DB2A8BB74F}"/>
-    <hyperlink ref="Q95" r:id="rId6" xr:uid="{3C7E4C22-E004-1E43-B5DA-014A2C03296E}"/>
+    <hyperlink ref="Q94" r:id="rId6" xr:uid="{3C7E4C22-E004-1E43-B5DA-014A2C03296E}"/>
     <hyperlink ref="Q17" r:id="rId7" xr:uid="{A7432939-477A-3F42-AB2E-D2FC38500BB0}"/>
     <hyperlink ref="Q125" r:id="rId8" xr:uid="{84961CAD-06D7-FA4C-986E-E6A3B93C66C9}"/>
     <hyperlink ref="Q115" r:id="rId9" xr:uid="{85627334-1CB7-9D43-B832-FB913FB4E7E4}"/>
@@ -15213,7 +15731,7 @@
     <hyperlink ref="Q152" r:id="rId76" xr:uid="{9CCB06D8-A39C-0649-AA09-D83FD1592BC5}"/>
     <hyperlink ref="Q188" r:id="rId77" xr:uid="{287782BB-04F0-0F49-8E68-94AFB58FDAEB}"/>
     <hyperlink ref="Q128" r:id="rId78" xr:uid="{6E798C00-5591-8D4C-8137-7896DE6E1F1A}"/>
-    <hyperlink ref="Q96" r:id="rId79" xr:uid="{584B5458-E2FC-444F-90EE-1CCB33F77375}"/>
+    <hyperlink ref="Q244" r:id="rId79" xr:uid="{584B5458-E2FC-444F-90EE-1CCB33F77375}"/>
     <hyperlink ref="Q129" r:id="rId80" xr:uid="{3E12F086-04A8-9E43-BE61-7BBC06FFB569}"/>
     <hyperlink ref="Q135" r:id="rId81" xr:uid="{418CB6F6-7582-1949-B8DB-B76A0557D620}"/>
     <hyperlink ref="Q187" r:id="rId82" xr:uid="{675E8E68-7CF3-4143-B1FC-1545455815E7}"/>
@@ -15225,15 +15743,15 @@
     <hyperlink ref="Q18" r:id="rId88" xr:uid="{9AE43FE7-D389-7045-80DB-B92387B3F9FC}"/>
     <hyperlink ref="Q154" r:id="rId89" xr:uid="{707E0CC3-8597-3544-BFCA-B6AFD8937A11}"/>
     <hyperlink ref="Q138" r:id="rId90" xr:uid="{1B0AF018-C249-F849-B489-83D881250376}"/>
-    <hyperlink ref="Q86" r:id="rId91" xr:uid="{425B7113-ACFE-3149-8C2F-01C9B2D8E631}"/>
+    <hyperlink ref="Q85" r:id="rId91" xr:uid="{425B7113-ACFE-3149-8C2F-01C9B2D8E631}"/>
     <hyperlink ref="Q51" r:id="rId92" xr:uid="{D4BB0AC9-51E9-614E-A21C-997DD817F4AE}"/>
     <hyperlink ref="Q16" r:id="rId93" xr:uid="{8157AD0D-E645-9745-A6FE-914B4948D699}"/>
-    <hyperlink ref="Q83" r:id="rId94" xr:uid="{3EB09505-96EA-9044-AB9E-9DE8D96D58EF}"/>
+    <hyperlink ref="Q82" r:id="rId94" xr:uid="{3EB09505-96EA-9044-AB9E-9DE8D96D58EF}"/>
     <hyperlink ref="Q66" r:id="rId95" xr:uid="{6AF79E23-C131-8F49-9524-0300598114A1}"/>
     <hyperlink ref="Q7" r:id="rId96" xr:uid="{FB2C0487-0616-AA4B-8932-A2C8EBCCAB5D}"/>
     <hyperlink ref="Q67" r:id="rId97" xr:uid="{FC820334-04F2-B74A-9535-FFE6FACA08F6}"/>
     <hyperlink ref="Q37" r:id="rId98" xr:uid="{36D36EC7-A52A-3C4E-91F3-719750EC6EE7}"/>
-    <hyperlink ref="Q78" r:id="rId99" xr:uid="{66BF9FB4-44C0-B641-817E-9F5FA438BC6E}"/>
+    <hyperlink ref="Q77" r:id="rId99" xr:uid="{66BF9FB4-44C0-B641-817E-9F5FA438BC6E}"/>
     <hyperlink ref="Q145" r:id="rId100" xr:uid="{A1FB719C-FEE4-8745-8EC3-B5A62EE0E44E}"/>
     <hyperlink ref="Q33" r:id="rId101" xr:uid="{54B22F91-320C-7F4A-A404-C7B7C4BE8F0A}"/>
     <hyperlink ref="Q166" r:id="rId102" xr:uid="{59E2FD0B-923D-3C42-8D05-1469557BDF68}"/>
@@ -15248,7 +15766,7 @@
     <hyperlink ref="Q47" r:id="rId111" xr:uid="{0AF73A99-F03F-CA42-B0E0-5D1B5C41F133}"/>
     <hyperlink ref="Q27" r:id="rId112" xr:uid="{E08FB853-7081-2A4C-B606-6E031C7423BB}"/>
     <hyperlink ref="Q199" r:id="rId113" xr:uid="{14CFFB1C-FCBC-6B4A-82E6-0193947BBD5D}"/>
-    <hyperlink ref="Q79" r:id="rId114" xr:uid="{4C5912D0-5972-7C4F-973E-8B0E87926534}"/>
+    <hyperlink ref="Q78" r:id="rId114" xr:uid="{4C5912D0-5972-7C4F-973E-8B0E87926534}"/>
     <hyperlink ref="Q202" r:id="rId115" xr:uid="{B10ED486-0ADE-AE45-920D-FAC73C4AA860}"/>
     <hyperlink ref="Q206" r:id="rId116" xr:uid="{CB8136AE-839D-214E-81C9-21399BA363BB}"/>
     <hyperlink ref="Q203" r:id="rId117" xr:uid="{0ECD14C3-3FA9-DF47-AB14-A9EE26B98ADB}"/>
@@ -15262,7 +15780,7 @@
     <hyperlink ref="Q73" r:id="rId125" xr:uid="{746FAB7B-FED8-F245-9FAB-1F5B1CCBAF43}"/>
     <hyperlink ref="Q56" r:id="rId126" xr:uid="{8134279C-1DCF-3D42-B28B-2D24B5A0103E}"/>
     <hyperlink ref="Q68" r:id="rId127" xr:uid="{22E6B370-27F9-0E49-8CA5-6758D6E54579}"/>
-    <hyperlink ref="Q80" r:id="rId128" xr:uid="{1C446669-E5AB-8D4D-9123-31185050C640}"/>
+    <hyperlink ref="Q79" r:id="rId128" xr:uid="{1C446669-E5AB-8D4D-9123-31185050C640}"/>
     <hyperlink ref="Q22" r:id="rId129" xr:uid="{44A33D6F-43C4-0943-BCB1-AF9DE4C147F6}"/>
     <hyperlink ref="Q55" r:id="rId130" xr:uid="{E02BB8E3-0BAF-C248-8EB0-3267BA432805}"/>
     <hyperlink ref="Q62" r:id="rId131" xr:uid="{BEFDCC98-9BB2-3D49-BA3F-3405DCD9093D}"/>
@@ -15272,30 +15790,30 @@
     <hyperlink ref="Q214" r:id="rId135" xr:uid="{3F83EA70-AEE6-8846-8419-3AD79B91EB73}"/>
     <hyperlink ref="Q70" r:id="rId136" xr:uid="{507E6A3E-3B2F-AF47-ACC6-43771B66EC1D}"/>
     <hyperlink ref="Q71" r:id="rId137" xr:uid="{F364D77A-F209-8646-B101-E1A004033D75}"/>
-    <hyperlink ref="Q99" r:id="rId138" xr:uid="{E488BDF2-FD76-C345-8345-C514E887B30D}"/>
+    <hyperlink ref="Q245" r:id="rId138" xr:uid="{E488BDF2-FD76-C345-8345-C514E887B30D}"/>
     <hyperlink ref="Q208" r:id="rId139" xr:uid="{3A350AA0-18E0-7A44-A617-2A23437C2D25}"/>
     <hyperlink ref="Q211" r:id="rId140" xr:uid="{2CD84B76-BD07-7447-AC85-335724F45069}"/>
     <hyperlink ref="Q212" r:id="rId141" xr:uid="{0D96B428-C157-194F-BBBB-55BACE11480C}"/>
-    <hyperlink ref="Q75" r:id="rId142" xr:uid="{68D7FE1B-2DB0-F244-9889-DBC0EF941E62}"/>
-    <hyperlink ref="Q77" r:id="rId143" xr:uid="{403EE16A-EAA6-E740-9294-3EE13C6F53DA}"/>
-    <hyperlink ref="Q74" r:id="rId144" xr:uid="{D699E543-EEDE-A143-BA28-8379A14B5C1E}"/>
+    <hyperlink ref="Q74" r:id="rId142" xr:uid="{68D7FE1B-2DB0-F244-9889-DBC0EF941E62}"/>
+    <hyperlink ref="Q75" r:id="rId143" xr:uid="{403EE16A-EAA6-E740-9294-3EE13C6F53DA}"/>
+    <hyperlink ref="Q104" r:id="rId144" xr:uid="{D699E543-EEDE-A143-BA28-8379A14B5C1E}"/>
     <hyperlink ref="Q210" r:id="rId145" xr:uid="{3D5A2B0F-23B9-7B48-B38D-6F0A511BA329}"/>
     <hyperlink ref="Q193" r:id="rId146" xr:uid="{ACAEC6C9-216A-534A-96A5-B91A6CBD58DD}"/>
-    <hyperlink ref="Q90" r:id="rId147" xr:uid="{3B49484B-4276-6241-AE6C-4768F1F60290}"/>
-    <hyperlink ref="Q82" r:id="rId148" xr:uid="{F9C03CE1-22DD-D449-B736-FFD2222FD11B}"/>
-    <hyperlink ref="Q92" r:id="rId149" xr:uid="{4312CDE6-A9CD-CB4F-954E-07A6504249E3}"/>
+    <hyperlink ref="Q89" r:id="rId147" xr:uid="{3B49484B-4276-6241-AE6C-4768F1F60290}"/>
+    <hyperlink ref="Q81" r:id="rId148" xr:uid="{F9C03CE1-22DD-D449-B736-FFD2222FD11B}"/>
+    <hyperlink ref="Q91" r:id="rId149" xr:uid="{4312CDE6-A9CD-CB4F-954E-07A6504249E3}"/>
     <hyperlink ref="Q63" r:id="rId150" xr:uid="{3EC4565A-606A-904D-A00D-7C065BC8A9CB}"/>
     <hyperlink ref="Q222" r:id="rId151" xr:uid="{11D1FB42-933A-D642-A0A9-1D751F8B8F73}"/>
     <hyperlink ref="Q223" r:id="rId152" xr:uid="{3AB784A4-BDB2-CF40-96CB-4EE5B7EB8ED2}"/>
     <hyperlink ref="Q224" r:id="rId153" xr:uid="{2352F29F-A1AD-2E44-B32C-934B4E87D28F}"/>
     <hyperlink ref="Q225" r:id="rId154" xr:uid="{8C880241-2719-8844-9AC7-9FD10D4835EE}"/>
-    <hyperlink ref="Q84" r:id="rId155" xr:uid="{9F1FE709-13B2-7542-B65F-1B593D0872D1}"/>
+    <hyperlink ref="Q83" r:id="rId155" xr:uid="{9F1FE709-13B2-7542-B65F-1B593D0872D1}"/>
     <hyperlink ref="Q215" r:id="rId156" xr:uid="{6917739B-949C-844A-A1B9-3BC57F6EA0CB}"/>
     <hyperlink ref="Q220" r:id="rId157" xr:uid="{22CD3B85-A12B-7940-A9D0-31167434C1F2}"/>
-    <hyperlink ref="Q91" r:id="rId158" xr:uid="{CF1362CC-10D9-464B-A4C2-4733A7A05746}"/>
-    <hyperlink ref="Q88" r:id="rId159" xr:uid="{60624615-A498-7B44-85E2-9675C84BE16F}"/>
-    <hyperlink ref="Q85" r:id="rId160" xr:uid="{BCE50138-0053-F442-92E8-958FA01416A1}"/>
-    <hyperlink ref="Q93" r:id="rId161" xr:uid="{3DEF2CF1-6AB5-6649-B66A-F141D76CC38F}"/>
+    <hyperlink ref="Q90" r:id="rId158" xr:uid="{CF1362CC-10D9-464B-A4C2-4733A7A05746}"/>
+    <hyperlink ref="Q87" r:id="rId159" xr:uid="{60624615-A498-7B44-85E2-9675C84BE16F}"/>
+    <hyperlink ref="Q84" r:id="rId160" xr:uid="{BCE50138-0053-F442-92E8-958FA01416A1}"/>
+    <hyperlink ref="Q92" r:id="rId161" xr:uid="{3DEF2CF1-6AB5-6649-B66A-F141D76CC38F}"/>
     <hyperlink ref="Q233" r:id="rId162" xr:uid="{13351AD9-151F-F84E-80D0-1B03FA8267C1}"/>
     <hyperlink ref="Q221" r:id="rId163" xr:uid="{20569A93-EB7A-4E47-A53B-8E5EDA719F82}"/>
     <hyperlink ref="Q231" r:id="rId164" xr:uid="{3E3EF4F9-D701-8E47-AE8A-BA3B863E5DF3}"/>
@@ -15306,12 +15824,18 @@
     <hyperlink ref="Q236" r:id="rId169" xr:uid="{26A12168-5A7B-7143-8285-FFDE7130F545}"/>
     <hyperlink ref="Q234" r:id="rId170" xr:uid="{98183D84-684A-5644-91AE-6881A42B6798}"/>
     <hyperlink ref="Q235" r:id="rId171" xr:uid="{FB65EF3E-1604-BA49-A777-BC22F86BA023}"/>
-    <hyperlink ref="B90" r:id="rId172" display="https://doi.org/10.20935/AL1274" xr:uid="{240C9844-798D-0B49-A453-CDA085161615}"/>
+    <hyperlink ref="B89" r:id="rId172" display="https://doi.org/10.20935/AL1274" xr:uid="{240C9844-798D-0B49-A453-CDA085161615}"/>
     <hyperlink ref="Q240" r:id="rId173" xr:uid="{1DFC1F7F-1957-B34C-A2D6-3630D0AF81F1}"/>
     <hyperlink ref="Q64" r:id="rId174" xr:uid="{07F1B89C-B381-984C-857C-4706FD61A432}"/>
     <hyperlink ref="Q243" r:id="rId175" xr:uid="{964D6BFA-35DA-834C-90ED-329D4CC344C2}"/>
-    <hyperlink ref="Q244" r:id="rId176" xr:uid="{FB0A5519-B7ED-FA4B-8017-6F734806C61F}"/>
-    <hyperlink ref="Q245" r:id="rId177" xr:uid="{031D270D-AE15-8F48-9950-82177BE16E1E}"/>
+    <hyperlink ref="Q101" r:id="rId176" xr:uid="{FB0A5519-B7ED-FA4B-8017-6F734806C61F}"/>
+    <hyperlink ref="Q103" r:id="rId177" xr:uid="{031D270D-AE15-8F48-9950-82177BE16E1E}"/>
+    <hyperlink ref="Q102" r:id="rId178" xr:uid="{B58C16B8-0C67-EC46-8FA2-669CBD477884}"/>
+    <hyperlink ref="Q249" r:id="rId179" xr:uid="{90345C85-218A-7945-97FC-0E6F4241CCC9}"/>
+    <hyperlink ref="Q250" r:id="rId180" xr:uid="{05A6C6B1-235B-5E4B-AE38-D43B4CCBE8D6}"/>
+    <hyperlink ref="Q252" r:id="rId181" xr:uid="{C32CB911-DC2F-1947-AB0C-5BAE829340DC}"/>
+    <hyperlink ref="Q254" r:id="rId182" xr:uid="{F26A7C8B-169A-6B48-8485-05BA0B48F7EB}"/>
+    <hyperlink ref="Q255" r:id="rId183" xr:uid="{E9ADE19D-E739-0140-80BE-AE3FB6DEA0AF}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updating with new pubs
</commit_message>
<xml_diff>
--- a/cv/cv_pubs.xlsx
+++ b/cv/cv_pubs.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/7_websites/doomlab_build/content/cv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/7_websites/cv_markdown_edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A262B8-95D1-484B-B329-22294025A72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18CB3AE-431D-1840-9DCD-C71DB95F18E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cv_pubs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cv_pubs!$A$1:$R$257</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cv_pubs!$A$1:$R$261</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2589" uniqueCount="1322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2627" uniqueCount="1341">
   <si>
     <t>title</t>
   </si>
@@ -3833,9 +3833,6 @@
     <t>XX-XX</t>
   </si>
   <si>
-    <t>Meaning, pandemic self-efficacy, social support, and discrimination predict trajectories of peri-pandemic growth and distress for international students</t>
-  </si>
-  <si>
     <t>https://www.aggieerin.com/pubs/Pavlacic_22_PT.docx</t>
   </si>
   <si>
@@ -3965,9 +3962,6 @@
     <t>u3T1itk59dMC</t>
   </si>
   <si>
-    <t>8VtEwCQfWZkC, XAp-VaTZjjwC, e84hm74t-eoC, uAPFzskPt0AC, oqD4_j7ulsYC, DQNrXyjhriIC</t>
-  </si>
-  <si>
     <t>Nature Scientific Data</t>
   </si>
   <si>
@@ -4002,6 +3996,69 @@
   </si>
   <si>
     <t>TBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.52041/serj.v21i3.29 </t>
+  </si>
+  <si>
+    <t>10.1016/j.dib.2022.108803</t>
+  </si>
+  <si>
+    <t>The Functional Assessment of Migraine Scale Development Datasets</t>
+  </si>
+  <si>
+    <t>Buchanan, E.M., Cady, R.J., Manley, H.R., Sly, J.S., \&amp; Wikowsky, A.</t>
+  </si>
+  <si>
+    <t>Data in Brief</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.dib.2022.108803</t>
+  </si>
+  <si>
+    <t>66133660, 121460393</t>
+  </si>
+  <si>
+    <t>10.1037/tra0001417</t>
+  </si>
+  <si>
+    <t>Perceived meaning, pandemic self-efficacy, social support, and discrimination predict trajectories of peri-pandemic growth and distress for international students</t>
+  </si>
+  <si>
+    <t>w2UhwfzvF0QC</t>
+  </si>
+  <si>
+    <t>10.31222/osf.io/rcews</t>
+  </si>
+  <si>
+    <t>Bochynska, A., et al.</t>
+  </si>
+  <si>
+    <t>https://osf.io/rcews</t>
+  </si>
+  <si>
+    <t>8VtEwCQfWZkC, XAp-VaTZjjwC, e84hm74t-eoC, uAPFzskPt0AC, oqD4_j7ulsYC, DQNrXyjhriIC, gV6rEsy15s0C</t>
+  </si>
+  <si>
+    <t>We don't know what you did last summer. On the importance of transparent reporting of reaction time data pre-processing</t>
+  </si>
+  <si>
+    <t>Loenneker, H., et al.</t>
+  </si>
+  <si>
+    <t>qCpRzq7zkD8C</t>
+  </si>
+  <si>
+    <t>10.31234/osf.io/tgzdk</t>
+  </si>
+  <si>
+    <t>https://osf.io/tgzdk</t>
+  </si>
+  <si>
+    <t>Predicting the replicability of social and behavioral science claims from the COVID 19 Preprint Replication Project with structured expert and novice groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcoci, A., et al. </t>
   </si>
 </sst>
 </file>
@@ -5005,11 +5062,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R257"/>
+  <dimension ref="A1:R261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q247" sqref="Q247"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="44.1640625" defaultRowHeight="16"/>
@@ -9737,7 +9794,7 @@
         <v>2022</v>
       </c>
       <c r="K93" t="s">
-        <v>1309</v>
+        <v>1333</v>
       </c>
       <c r="M93" s="1" t="s">
         <v>179</v>
@@ -9819,7 +9876,7 @@
         <v>1</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>1259</v>
@@ -9849,7 +9906,7 @@
         <v>1206</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="M95" s="1" t="s">
         <v>179</v>
@@ -9927,6 +9984,9 @@
       <c r="A97" s="16">
         <v>1</v>
       </c>
+      <c r="B97" s="1" t="s">
+        <v>1320</v>
+      </c>
       <c r="C97" s="1" t="s">
         <v>1113</v>
       </c>
@@ -9939,14 +9999,14 @@
       <c r="F97" s="1" t="s">
         <v>1247</v>
       </c>
-      <c r="G97" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>178</v>
+      <c r="G97" s="1">
+        <v>21</v>
+      </c>
+      <c r="H97" s="1">
+        <v>3</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="J97" s="1">
         <v>2022</v>
@@ -10023,7 +10083,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>1150</v>
@@ -10041,13 +10101,13 @@
         <v>3</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="J99" s="1">
         <v>2022</v>
       </c>
       <c r="K99" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="M99" s="1" t="s">
         <v>179</v>
@@ -10122,7 +10182,7 @@
         <v>7</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="J101" s="1">
         <v>2022</v>
@@ -10152,12 +10212,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="102" spans="1:18" ht="51">
+    <row r="102" spans="1:18" ht="68">
       <c r="A102" s="16">
         <v>1</v>
       </c>
+      <c r="B102" s="1" t="s">
+        <v>1327</v>
+      </c>
       <c r="C102" s="8" t="s">
-        <v>1265</v>
+        <v>1328</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>1148</v>
@@ -10175,7 +10238,13 @@
         <v>274</v>
       </c>
       <c r="J102" s="1">
-        <v>2022</v>
+        <v>2023</v>
+      </c>
+      <c r="K102" t="s">
+        <v>1329</v>
+      </c>
+      <c r="L102">
+        <v>126109116</v>
       </c>
       <c r="M102" s="1" t="s">
         <v>179</v>
@@ -10190,7 +10259,7 @@
         <v>195</v>
       </c>
       <c r="Q102" s="2" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="R102" s="1">
         <v>81</v>
@@ -10216,7 +10285,7 @@
         <v>26</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J103" s="1">
         <v>2022</v>
@@ -10247,7 +10316,7 @@
       <c r="A104" s="16">
         <v>1</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" t="s">
         <v>1262</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -10277,8 +10346,8 @@
       <c r="K104" t="s">
         <v>966</v>
       </c>
-      <c r="L104">
-        <v>66133660</v>
+      <c r="L104" t="s">
+        <v>1326</v>
       </c>
       <c r="M104" s="1" t="s">
         <v>179</v>
@@ -15034,7 +15103,7 @@
         <v>195</v>
       </c>
       <c r="Q238" s="2" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="R238" s="1"/>
     </row>
@@ -15067,7 +15136,7 @@
         <v>195</v>
       </c>
       <c r="Q239" s="2" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="R239" s="1"/>
     </row>
@@ -15186,7 +15255,7 @@
         <v>1182</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="G243" s="1" t="s">
         <v>178</v>
@@ -15318,16 +15387,16 @@
         <v>1</v>
       </c>
       <c r="C246" s="29" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E246" s="1" t="s">
         <v>1267</v>
       </c>
-      <c r="E246" s="1" t="s">
+      <c r="F246" s="1" t="s">
         <v>1268</v>
       </c>
-      <c r="F246" s="1" t="s">
+      <c r="J246" s="1" t="s">
         <v>1269</v>
-      </c>
-      <c r="J246" s="1" t="s">
-        <v>1270</v>
       </c>
       <c r="M246" s="1" t="s">
         <v>215</v>
@@ -15342,7 +15411,7 @@
         <v>195</v>
       </c>
       <c r="Q246" s="1" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="247" spans="1:18" ht="51">
@@ -15350,16 +15419,16 @@
         <v>1</v>
       </c>
       <c r="C247" s="28" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="E247" s="30" t="s">
         <v>1118</v>
       </c>
       <c r="F247" s="1" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="J247" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="M247" s="1" t="s">
         <v>215</v>
@@ -15374,7 +15443,7 @@
         <v>185</v>
       </c>
       <c r="Q247" s="2" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="248" spans="1:18" ht="34">
@@ -15382,16 +15451,16 @@
         <v>1</v>
       </c>
       <c r="C248" s="28" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="E248" s="30" t="s">
+        <v>1272</v>
+      </c>
+      <c r="F248" s="1" t="s">
         <v>1273</v>
       </c>
-      <c r="F248" s="1" t="s">
-        <v>1274</v>
-      </c>
       <c r="J248" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="M248" s="1" t="s">
         <v>215</v>
@@ -15406,7 +15475,7 @@
         <v>185</v>
       </c>
       <c r="Q248" s="2" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="249" spans="1:18" ht="51">
@@ -15414,16 +15483,16 @@
         <v>1</v>
       </c>
       <c r="C249" s="28" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="E249" s="30" t="s">
         <v>207</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="J249" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="M249" s="1" t="s">
         <v>215</v>
@@ -15438,7 +15507,7 @@
         <v>195</v>
       </c>
       <c r="Q249" s="2" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="250" spans="1:18" ht="34">
@@ -15446,16 +15515,16 @@
         <v>1</v>
       </c>
       <c r="C250" s="28" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E250" s="30" t="s">
         <v>207</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="J250" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="M250" s="1" t="s">
         <v>215</v>
@@ -15470,7 +15539,7 @@
         <v>185</v>
       </c>
       <c r="Q250" s="2" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="251" spans="1:18" ht="34">
@@ -15478,16 +15547,16 @@
         <v>1</v>
       </c>
       <c r="C251" s="28" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>207</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="J251" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="M251" s="1" t="s">
         <v>215</v>
@@ -15502,7 +15571,7 @@
         <v>195</v>
       </c>
       <c r="Q251" s="2" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="252" spans="1:18" ht="34">
@@ -15510,16 +15579,16 @@
         <v>1</v>
       </c>
       <c r="C252" s="28" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="E252" s="1" t="s">
         <v>207</v>
       </c>
       <c r="F252" s="1" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="J252" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="M252" s="1" t="s">
         <v>215</v>
@@ -15534,7 +15603,7 @@
         <v>195</v>
       </c>
       <c r="Q252" s="2" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="253" spans="1:18" ht="34">
@@ -15542,16 +15611,16 @@
         <v>1</v>
       </c>
       <c r="C253" s="28" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="E253" s="1" t="s">
         <v>207</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="J253" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="M253" s="1" t="s">
         <v>215</v>
@@ -15566,7 +15635,7 @@
         <v>185</v>
       </c>
       <c r="Q253" s="2" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="254" spans="1:18" ht="34">
@@ -15574,16 +15643,16 @@
         <v>1</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="E254" s="1" t="s">
         <v>1166</v>
       </c>
       <c r="F254" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="J254" s="1" t="s">
         <v>1289</v>
-      </c>
-      <c r="J254" s="1" t="s">
-        <v>1290</v>
       </c>
       <c r="M254" s="1" t="s">
         <v>215</v>
@@ -15598,7 +15667,7 @@
         <v>195</v>
       </c>
       <c r="Q254" s="2" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="255" spans="1:18" ht="51">
@@ -15606,16 +15675,16 @@
         <v>1</v>
       </c>
       <c r="C255" s="1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E255" s="1" t="s">
         <v>1291</v>
       </c>
-      <c r="E255" s="1" t="s">
+      <c r="F255" s="1" t="s">
         <v>1292</v>
       </c>
-      <c r="F255" s="1" t="s">
+      <c r="J255" s="1" t="s">
         <v>1293</v>
-      </c>
-      <c r="J255" s="1" t="s">
-        <v>1294</v>
       </c>
       <c r="M255" s="1" t="s">
         <v>215</v>
@@ -15630,7 +15699,7 @@
         <v>195</v>
       </c>
       <c r="Q255" s="2" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="256" spans="1:18" ht="34">
@@ -15638,16 +15707,16 @@
         <v>1</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E256" s="1" t="s">
         <v>1166</v>
       </c>
       <c r="F256" s="1" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="J256" s="1" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="M256" s="1" t="s">
         <v>215</v>
@@ -15662,27 +15731,27 @@
         <v>185</v>
       </c>
       <c r="Q256" s="2" t="s">
-        <v>1297</v>
-      </c>
-    </row>
-    <row r="257" spans="1:17" ht="68">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="257" spans="1:18" ht="68">
       <c r="A257" s="16">
         <v>1</v>
       </c>
       <c r="C257" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E257" s="1" t="s">
         <v>1303</v>
-      </c>
-      <c r="E257" s="1" t="s">
-        <v>1304</v>
       </c>
       <c r="J257" s="1">
         <v>2022</v>
       </c>
       <c r="K257" s="1" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="M257" s="1" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="N257" s="1" t="s">
         <v>200</v>
@@ -15694,7 +15763,162 @@
         <v>195</v>
       </c>
       <c r="Q257" s="1" t="s">
-        <v>1306</v>
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="258" spans="1:18" ht="34">
+      <c r="A258" s="16">
+        <v>1</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="G258" s="1">
+        <v>46</v>
+      </c>
+      <c r="H258" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I258">
+        <v>108803</v>
+      </c>
+      <c r="J258" s="1">
+        <v>2023</v>
+      </c>
+      <c r="K258" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="M258" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N258" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O258" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P258" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q258" s="2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="R258" s="8">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="259" spans="1:18" ht="34">
+      <c r="A259" s="16">
+        <v>1</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>1331</v>
+      </c>
+      <c r="J259" s="1">
+        <v>2023</v>
+      </c>
+      <c r="K259" t="s">
+        <v>1216</v>
+      </c>
+      <c r="L259">
+        <v>126336455</v>
+      </c>
+      <c r="M259" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N259" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O259" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P259" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q259" s="2" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="260" spans="1:18" ht="51">
+      <c r="A260" s="16">
+        <v>1</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>1337</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>1335</v>
+      </c>
+      <c r="J260" s="1">
+        <v>2023</v>
+      </c>
+      <c r="K260" t="s">
+        <v>1336</v>
+      </c>
+      <c r="L260">
+        <v>125625045</v>
+      </c>
+      <c r="M260" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N260" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O260" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P260" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q260" s="2" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="261" spans="1:18" ht="68">
+      <c r="A261" s="16">
+        <v>1</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>1339</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>1340</v>
+      </c>
+      <c r="J261" s="1">
+        <v>2023</v>
+      </c>
+      <c r="M261" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N261" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O261" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P261" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q261" s="1" t="s">
+        <v>1319</v>
       </c>
     </row>
   </sheetData>
@@ -15901,6 +16125,9 @@
     <hyperlink ref="Q252" r:id="rId188" xr:uid="{72E6E786-291C-874D-AA75-878577703733}"/>
     <hyperlink ref="Q248" r:id="rId189" xr:uid="{CCB5C3CC-A0A8-DF4C-8FA7-A989BFCA7E7D}"/>
     <hyperlink ref="Q247" r:id="rId190" xr:uid="{23185960-6CE5-8741-B85B-A11162ED99D9}"/>
+    <hyperlink ref="Q258" r:id="rId191" xr:uid="{89DF0D51-3963-0242-9050-B48506698F57}"/>
+    <hyperlink ref="Q259" r:id="rId192" xr:uid="{BE84FD2D-9113-F34C-9AA1-EF7278924714}"/>
+    <hyperlink ref="Q260" r:id="rId193" xr:uid="{8D80FEC9-D23B-D647-BD8F-8AA2B650036E}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>